<commit_message>
Remove commas in cells in web-app/BCF
</commit_message>
<xml_diff>
--- a/InputData/web-app/BCF/BTU Conversion Factors.xlsx
+++ b/InputData/web-app/BCF/BTU Conversion Factors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\web-app\BCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\web-app\BCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3468,7 +3468,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="211">
+  <cellXfs count="209">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3867,11 +3867,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="63">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4270,9 +4268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4636,7 +4632,7 @@
       <selection activeCell="C32" sqref="C32"/>
       <selection pane="topRight" activeCell="C32" sqref="C32"/>
       <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
-      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11275,44 +11271,44 @@
     </row>
     <row r="77" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="209" t="s">
+      <c r="B78" s="208" t="s">
         <v>57</v>
       </c>
-      <c r="C78" s="209"/>
-      <c r="D78" s="209"/>
-      <c r="E78" s="209"/>
-      <c r="F78" s="209"/>
-      <c r="G78" s="209"/>
-      <c r="H78" s="209"/>
-      <c r="I78" s="209"/>
-      <c r="J78" s="209"/>
-      <c r="K78" s="209"/>
-      <c r="L78" s="209"/>
-      <c r="M78" s="209"/>
-      <c r="N78" s="209"/>
-      <c r="O78" s="209"/>
-      <c r="P78" s="209"/>
-      <c r="Q78" s="209"/>
-      <c r="R78" s="209"/>
-      <c r="S78" s="209"/>
-      <c r="T78" s="209"/>
-      <c r="U78" s="209"/>
-      <c r="V78" s="209"/>
-      <c r="W78" s="209"/>
-      <c r="X78" s="209"/>
-      <c r="Y78" s="209"/>
-      <c r="Z78" s="209"/>
-      <c r="AA78" s="209"/>
-      <c r="AB78" s="209"/>
-      <c r="AC78" s="209"/>
-      <c r="AD78" s="209"/>
-      <c r="AE78" s="209"/>
-      <c r="AF78" s="209"/>
-      <c r="AG78" s="209"/>
-      <c r="AH78" s="209"/>
-      <c r="AI78" s="209"/>
-      <c r="AJ78" s="209"/>
-      <c r="AK78" s="209"/>
+      <c r="C78" s="208"/>
+      <c r="D78" s="208"/>
+      <c r="E78" s="208"/>
+      <c r="F78" s="208"/>
+      <c r="G78" s="208"/>
+      <c r="H78" s="208"/>
+      <c r="I78" s="208"/>
+      <c r="J78" s="208"/>
+      <c r="K78" s="208"/>
+      <c r="L78" s="208"/>
+      <c r="M78" s="208"/>
+      <c r="N78" s="208"/>
+      <c r="O78" s="208"/>
+      <c r="P78" s="208"/>
+      <c r="Q78" s="208"/>
+      <c r="R78" s="208"/>
+      <c r="S78" s="208"/>
+      <c r="T78" s="208"/>
+      <c r="U78" s="208"/>
+      <c r="V78" s="208"/>
+      <c r="W78" s="208"/>
+      <c r="X78" s="208"/>
+      <c r="Y78" s="208"/>
+      <c r="Z78" s="208"/>
+      <c r="AA78" s="208"/>
+      <c r="AB78" s="208"/>
+      <c r="AC78" s="208"/>
+      <c r="AD78" s="208"/>
+      <c r="AE78" s="208"/>
+      <c r="AF78" s="208"/>
+      <c r="AG78" s="208"/>
+      <c r="AH78" s="208"/>
+      <c r="AI78" s="208"/>
+      <c r="AJ78" s="208"/>
+      <c r="AK78" s="208"/>
     </row>
     <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="8" t="s">
@@ -11362,9 +11358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X163"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
-    </sheetView>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15856,9 +15850,7 @@
   </sheetPr>
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:AI22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18811,9 +18803,7 @@
   </sheetPr>
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19818,139 +19808,139 @@
       <c r="A9" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B9" s="210">
+      <c r="B9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="C9" s="210">
+      <c r="C9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="D9" s="210">
+      <c r="D9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="E9" s="210">
+      <c r="E9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="F9" s="210">
+      <c r="F9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="G9" s="210">
+      <c r="G9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="H9" s="210">
+      <c r="H9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="I9" s="210">
+      <c r="I9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="J9" s="210">
+      <c r="J9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="K9" s="210">
+      <c r="K9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="L9" s="210">
+      <c r="L9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="M9" s="210">
+      <c r="M9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="N9" s="210">
+      <c r="N9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="O9" s="210">
+      <c r="O9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="P9" s="210">
+      <c r="P9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="Q9" s="210">
+      <c r="Q9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="R9" s="210">
+      <c r="R9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="S9" s="210">
+      <c r="S9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="T9" s="210">
+      <c r="T9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="U9" s="210">
+      <c r="U9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="V9" s="210">
+      <c r="V9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="W9" s="210">
+      <c r="W9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="X9" s="210">
+      <c r="X9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="Y9" s="210">
+      <c r="Y9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="Z9" s="210">
+      <c r="Z9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="AA9" s="210">
+      <c r="AA9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="AB9" s="210">
+      <c r="AB9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="AC9" s="210">
+      <c r="AC9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="AD9" s="210">
+      <c r="AD9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="AE9" s="210">
+      <c r="AE9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="AF9" s="210">
+      <c r="AF9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="AG9" s="210">
+      <c r="AG9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="AH9" s="210">
+      <c r="AH9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
-      <c r="AI9" s="210">
+      <c r="AI9" s="5">
         <f>'GREET1 Fuel_Specs'!$D$81</f>
         <v>17906000</v>
       </c>
@@ -19959,139 +19949,139 @@
       <c r="A10" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B10" s="208">
+      <c r="B10" s="5">
         <f>'AEO Table 73'!C32*10^6/gal_per_barrel</f>
         <v>120396.26190476191</v>
       </c>
-      <c r="C10" s="208">
+      <c r="C10" s="5">
         <f>'AEO Table 73'!D32*10^6/gal_per_barrel</f>
         <v>120363.33333333333</v>
       </c>
-      <c r="D10" s="208">
+      <c r="D10" s="5">
         <f>'AEO Table 73'!E32*10^6/gal_per_barrel</f>
         <v>120379.16666666667</v>
       </c>
-      <c r="E10" s="208">
+      <c r="E10" s="5">
         <f>'AEO Table 73'!F32*10^6/gal_per_barrel</f>
         <v>120387.38095238095</v>
       </c>
-      <c r="F10" s="208">
+      <c r="F10" s="5">
         <f>'AEO Table 73'!G32*10^6/gal_per_barrel</f>
         <v>120365.73809523809</v>
       </c>
-      <c r="G10" s="208">
+      <c r="G10" s="5">
         <f>'AEO Table 73'!H32*10^6/gal_per_barrel</f>
         <v>120317.52380952382</v>
       </c>
-      <c r="H10" s="208">
+      <c r="H10" s="5">
         <f>'AEO Table 73'!I32*10^6/gal_per_barrel</f>
         <v>120257.52380952382</v>
       </c>
-      <c r="I10" s="208">
+      <c r="I10" s="5">
         <f>'AEO Table 73'!J32*10^6/gal_per_barrel</f>
         <v>120238.14285714286</v>
       </c>
-      <c r="J10" s="208">
+      <c r="J10" s="5">
         <f>'AEO Table 73'!K32*10^6/gal_per_barrel</f>
         <v>120225.69047619047</v>
       </c>
-      <c r="K10" s="208">
+      <c r="K10" s="5">
         <f>'AEO Table 73'!L32*10^6/gal_per_barrel</f>
         <v>120215.88095238095</v>
       </c>
-      <c r="L10" s="208">
+      <c r="L10" s="5">
         <f>'AEO Table 73'!M32*10^6/gal_per_barrel</f>
         <v>120205.23809523809</v>
       </c>
-      <c r="M10" s="208">
+      <c r="M10" s="5">
         <f>'AEO Table 73'!N32*10^6/gal_per_barrel</f>
         <v>120194.90476190476</v>
       </c>
-      <c r="N10" s="208">
+      <c r="N10" s="5">
         <f>'AEO Table 73'!O32*10^6/gal_per_barrel</f>
         <v>120184.57142857143</v>
       </c>
-      <c r="O10" s="208">
+      <c r="O10" s="5">
         <f>'AEO Table 73'!P32*10^6/gal_per_barrel</f>
         <v>120186.35714285714</v>
       </c>
-      <c r="P10" s="208">
+      <c r="P10" s="5">
         <f>'AEO Table 73'!Q32*10^6/gal_per_barrel</f>
         <v>120169.33333333333</v>
       </c>
-      <c r="Q10" s="208">
+      <c r="Q10" s="5">
         <f>'AEO Table 73'!R32*10^6/gal_per_barrel</f>
         <v>120159.80952380953</v>
       </c>
-      <c r="R10" s="208">
+      <c r="R10" s="5">
         <f>'AEO Table 73'!S32*10^6/gal_per_barrel</f>
         <v>120153.90476190476</v>
       </c>
-      <c r="S10" s="208">
+      <c r="S10" s="5">
         <f>'AEO Table 73'!T32*10^6/gal_per_barrel</f>
         <v>120139.92857142857</v>
       </c>
-      <c r="T10" s="208">
+      <c r="T10" s="5">
         <f>'AEO Table 73'!U32*10^6/gal_per_barrel</f>
         <v>120123.47619047618</v>
       </c>
-      <c r="U10" s="208">
+      <c r="U10" s="5">
         <f>'AEO Table 73'!V32*10^6/gal_per_barrel</f>
         <v>120105.47619047618</v>
       </c>
-      <c r="V10" s="208">
+      <c r="V10" s="5">
         <f>'AEO Table 73'!W32*10^6/gal_per_barrel</f>
         <v>120085.26190476191</v>
       </c>
-      <c r="W10" s="208">
+      <c r="W10" s="5">
         <f>'AEO Table 73'!X32*10^6/gal_per_barrel</f>
         <v>120065.59523809524</v>
       </c>
-      <c r="X10" s="208">
+      <c r="X10" s="5">
         <f>'AEO Table 73'!Y32*10^6/gal_per_barrel</f>
         <v>120040.19047619047</v>
       </c>
-      <c r="Y10" s="208">
+      <c r="Y10" s="5">
         <f>'AEO Table 73'!Z32*10^6/gal_per_barrel</f>
         <v>120011.85714285714</v>
       </c>
-      <c r="Z10" s="208">
+      <c r="Z10" s="5">
         <f>'AEO Table 73'!AA32*10^6/gal_per_barrel</f>
         <v>119980</v>
       </c>
-      <c r="AA10" s="208">
+      <c r="AA10" s="5">
         <f>'AEO Table 73'!AB32*10^6/gal_per_barrel</f>
         <v>119949.21428571429</v>
       </c>
-      <c r="AB10" s="208">
+      <c r="AB10" s="5">
         <f>'AEO Table 73'!AC32*10^6/gal_per_barrel</f>
         <v>119910.09523809524</v>
       </c>
-      <c r="AC10" s="208">
+      <c r="AC10" s="5">
         <f>'AEO Table 73'!AD32*10^6/gal_per_barrel</f>
         <v>119871.47619047618</v>
       </c>
-      <c r="AD10" s="208">
+      <c r="AD10" s="5">
         <f>'AEO Table 73'!AE32*10^6/gal_per_barrel</f>
         <v>119830.30952380953</v>
       </c>
-      <c r="AE10" s="208">
+      <c r="AE10" s="5">
         <f>'AEO Table 73'!AF32*10^6/gal_per_barrel</f>
         <v>119784.40476190476</v>
       </c>
-      <c r="AF10" s="208">
+      <c r="AF10" s="5">
         <f>'AEO Table 73'!AG32*10^6/gal_per_barrel</f>
         <v>119727.33333333333</v>
       </c>
-      <c r="AG10" s="208">
+      <c r="AG10" s="5">
         <f>'AEO Table 73'!AH32*10^6/gal_per_barrel</f>
         <v>119664.71428571429</v>
       </c>
-      <c r="AH10" s="208">
+      <c r="AH10" s="5">
         <f>'AEO Table 73'!AI32*10^6/gal_per_barrel</f>
         <v>119596.14285714286</v>
       </c>
-      <c r="AI10" s="208">
+      <c r="AI10" s="5">
         <f>'AEO Table 73'!AJ32*10^6/gal_per_barrel</f>
         <v>119596.09523809524</v>
       </c>
@@ -20100,139 +20090,139 @@
       <c r="A11" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B11" s="208">
+      <c r="B11" s="5">
         <f>'AEO Table 73'!C19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="C11" s="208">
+      <c r="C11" s="5">
         <f>'AEO Table 73'!D19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="D11" s="208">
+      <c r="D11" s="5">
         <f>'AEO Table 73'!E19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="E11" s="208">
+      <c r="E11" s="5">
         <f>'AEO Table 73'!F19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="F11" s="208">
+      <c r="F11" s="5">
         <f>'AEO Table 73'!G19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="G11" s="208">
+      <c r="G11" s="5">
         <f>'AEO Table 73'!H19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="H11" s="208">
+      <c r="H11" s="5">
         <f>'AEO Table 73'!I19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="I11" s="208">
+      <c r="I11" s="5">
         <f>'AEO Table 73'!J19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="J11" s="208">
+      <c r="J11" s="5">
         <f>'AEO Table 73'!K19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="K11" s="208">
+      <c r="K11" s="5">
         <f>'AEO Table 73'!L19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="L11" s="208">
+      <c r="L11" s="5">
         <f>'AEO Table 73'!M19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="M11" s="208">
+      <c r="M11" s="5">
         <f>'AEO Table 73'!N19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="N11" s="208">
+      <c r="N11" s="5">
         <f>'AEO Table 73'!O19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="O11" s="208">
+      <c r="O11" s="5">
         <f>'AEO Table 73'!P19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="P11" s="208">
+      <c r="P11" s="5">
         <f>'AEO Table 73'!Q19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="Q11" s="208">
+      <c r="Q11" s="5">
         <f>'AEO Table 73'!R19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="R11" s="208">
+      <c r="R11" s="5">
         <f>'AEO Table 73'!S19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="S11" s="208">
+      <c r="S11" s="5">
         <f>'AEO Table 73'!T19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="T11" s="208">
+      <c r="T11" s="5">
         <f>'AEO Table 73'!U19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="U11" s="208">
+      <c r="U11" s="5">
         <f>'AEO Table 73'!V19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="V11" s="208">
+      <c r="V11" s="5">
         <f>'AEO Table 73'!W19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="W11" s="208">
+      <c r="W11" s="5">
         <f>'AEO Table 73'!X19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="X11" s="208">
+      <c r="X11" s="5">
         <f>'AEO Table 73'!Y19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="Y11" s="208">
+      <c r="Y11" s="5">
         <f>'AEO Table 73'!Z19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="Z11" s="208">
+      <c r="Z11" s="5">
         <f>'AEO Table 73'!AA19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="AA11" s="208">
+      <c r="AA11" s="5">
         <f>'AEO Table 73'!AB19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="AB11" s="208">
+      <c r="AB11" s="5">
         <f>'AEO Table 73'!AC19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="AC11" s="208">
+      <c r="AC11" s="5">
         <f>'AEO Table 73'!AD19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="AD11" s="208">
+      <c r="AD11" s="5">
         <f>'AEO Table 73'!AE19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="AE11" s="208">
+      <c r="AE11" s="5">
         <f>'AEO Table 73'!AF19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="AF11" s="208">
+      <c r="AF11" s="5">
         <f>'AEO Table 73'!AG19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="AG11" s="208">
+      <c r="AG11" s="5">
         <f>'AEO Table 73'!AH19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="AH11" s="208">
+      <c r="AH11" s="5">
         <f>'AEO Table 73'!AI19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
-      <c r="AI11" s="208">
+      <c r="AI11" s="5">
         <f>'AEO Table 73'!AJ19*10^6/gal_per_barrel</f>
         <v>138690.47619047618</v>
       </c>
@@ -20241,139 +20231,139 @@
       <c r="A12" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B12" s="208">
+      <c r="B12" s="5">
         <f>'AEO Table 73'!C29*10^6/gal_per_barrel</f>
         <v>95171.904761904763</v>
       </c>
-      <c r="C12" s="208">
+      <c r="C12" s="5">
         <f>'AEO Table 73'!D29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="D12" s="208">
+      <c r="D12" s="5">
         <f>'AEO Table 73'!E29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="E12" s="208">
+      <c r="E12" s="5">
         <f>'AEO Table 73'!F29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="F12" s="208">
+      <c r="F12" s="5">
         <f>'AEO Table 73'!G29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="G12" s="208">
+      <c r="G12" s="5">
         <f>'AEO Table 73'!H29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="H12" s="208">
+      <c r="H12" s="5">
         <f>'AEO Table 73'!I29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="I12" s="208">
+      <c r="I12" s="5">
         <f>'AEO Table 73'!J29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="J12" s="208">
+      <c r="J12" s="5">
         <f>'AEO Table 73'!K29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="K12" s="208">
+      <c r="K12" s="5">
         <f>'AEO Table 73'!L29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="L12" s="208">
+      <c r="L12" s="5">
         <f>'AEO Table 73'!M29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="M12" s="208">
+      <c r="M12" s="5">
         <f>'AEO Table 73'!N29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="N12" s="208">
+      <c r="N12" s="5">
         <f>'AEO Table 73'!O29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="O12" s="208">
+      <c r="O12" s="5">
         <f>'AEO Table 73'!P29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="P12" s="208">
+      <c r="P12" s="5">
         <f>'AEO Table 73'!Q29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="Q12" s="208">
+      <c r="Q12" s="5">
         <f>'AEO Table 73'!R29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="R12" s="208">
+      <c r="R12" s="5">
         <f>'AEO Table 73'!S29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="S12" s="208">
+      <c r="S12" s="5">
         <f>'AEO Table 73'!T29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="T12" s="208">
+      <c r="T12" s="5">
         <f>'AEO Table 73'!U29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="U12" s="208">
+      <c r="U12" s="5">
         <f>'AEO Table 73'!V29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="V12" s="208">
+      <c r="V12" s="5">
         <f>'AEO Table 73'!W29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="W12" s="208">
+      <c r="W12" s="5">
         <f>'AEO Table 73'!X29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="X12" s="208">
+      <c r="X12" s="5">
         <f>'AEO Table 73'!Y29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="Y12" s="208">
+      <c r="Y12" s="5">
         <f>'AEO Table 73'!Z29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="Z12" s="208">
+      <c r="Z12" s="5">
         <f>'AEO Table 73'!AA29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="AA12" s="208">
+      <c r="AA12" s="5">
         <f>'AEO Table 73'!AB29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="AB12" s="208">
+      <c r="AB12" s="5">
         <f>'AEO Table 73'!AC29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="AC12" s="208">
+      <c r="AC12" s="5">
         <f>'AEO Table 73'!AD29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="AD12" s="208">
+      <c r="AD12" s="5">
         <f>'AEO Table 73'!AE29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="AE12" s="208">
+      <c r="AE12" s="5">
         <f>'AEO Table 73'!AF29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="AF12" s="208">
+      <c r="AF12" s="5">
         <f>'AEO Table 73'!AG29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="AG12" s="208">
+      <c r="AG12" s="5">
         <f>'AEO Table 73'!AH29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="AH12" s="208">
+      <c r="AH12" s="5">
         <f>'AEO Table 73'!AI29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
-      <c r="AI12" s="208">
+      <c r="AI12" s="5">
         <f>'AEO Table 73'!AJ29*10^6/gal_per_barrel</f>
         <v>94981.738095238092</v>
       </c>
@@ -20382,139 +20372,139 @@
       <c r="A13" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="B13" s="208">
+      <c r="B13" s="5">
         <f>'AEO Table 73'!C18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="C13" s="208">
+      <c r="C13" s="5">
         <f>'AEO Table 73'!D18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="D13" s="208">
+      <c r="D13" s="5">
         <f>'AEO Table 73'!E18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="E13" s="208">
+      <c r="E13" s="5">
         <f>'AEO Table 73'!F18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="F13" s="208">
+      <c r="F13" s="5">
         <f>'AEO Table 73'!G18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="G13" s="208">
+      <c r="G13" s="5">
         <f>'AEO Table 73'!H18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="H13" s="208">
+      <c r="H13" s="5">
         <f>'AEO Table 73'!I18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="I13" s="208">
+      <c r="I13" s="5">
         <f>'AEO Table 73'!J18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="J13" s="208">
+      <c r="J13" s="5">
         <f>'AEO Table 73'!K18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="K13" s="208">
+      <c r="K13" s="5">
         <f>'AEO Table 73'!L18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="L13" s="208">
+      <c r="L13" s="5">
         <f>'AEO Table 73'!M18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="M13" s="208">
+      <c r="M13" s="5">
         <f>'AEO Table 73'!N18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="N13" s="208">
+      <c r="N13" s="5">
         <f>'AEO Table 73'!O18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="O13" s="208">
+      <c r="O13" s="5">
         <f>'AEO Table 73'!P18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="P13" s="208">
+      <c r="P13" s="5">
         <f>'AEO Table 73'!Q18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="Q13" s="208">
+      <c r="Q13" s="5">
         <f>'AEO Table 73'!R18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="R13" s="208">
+      <c r="R13" s="5">
         <f>'AEO Table 73'!S18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="S13" s="208">
+      <c r="S13" s="5">
         <f>'AEO Table 73'!T18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="T13" s="208">
+      <c r="T13" s="5">
         <f>'AEO Table 73'!U18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="U13" s="208">
+      <c r="U13" s="5">
         <f>'AEO Table 73'!V18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="V13" s="208">
+      <c r="V13" s="5">
         <f>'AEO Table 73'!W18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="W13" s="208">
+      <c r="W13" s="5">
         <f>'AEO Table 73'!X18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="X13" s="208">
+      <c r="X13" s="5">
         <f>'AEO Table 73'!Y18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="Y13" s="208">
+      <c r="Y13" s="5">
         <f>'AEO Table 73'!Z18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="Z13" s="208">
+      <c r="Z13" s="5">
         <f>'AEO Table 73'!AA18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="AA13" s="208">
+      <c r="AA13" s="5">
         <f>'AEO Table 73'!AB18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="AB13" s="208">
+      <c r="AB13" s="5">
         <f>'AEO Table 73'!AC18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="AC13" s="208">
+      <c r="AC13" s="5">
         <f>'AEO Table 73'!AD18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="AD13" s="208">
+      <c r="AD13" s="5">
         <f>'AEO Table 73'!AE18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="AE13" s="208">
+      <c r="AE13" s="5">
         <f>'AEO Table 73'!AF18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="AF13" s="208">
+      <c r="AF13" s="5">
         <f>'AEO Table 73'!AG18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="AG13" s="208">
+      <c r="AG13" s="5">
         <f>'AEO Table 73'!AH18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="AH13" s="208">
+      <c r="AH13" s="5">
         <f>'AEO Table 73'!AI18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
-      <c r="AI13" s="208">
+      <c r="AI13" s="5">
         <f>'AEO Table 73'!AJ18*10^6/gal_per_barrel</f>
         <v>127595.23809523809</v>
       </c>
@@ -20912,139 +20902,139 @@
       <c r="A17" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B17" s="210">
+      <c r="B17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="C17" s="210">
+      <c r="C17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="D17" s="210">
+      <c r="D17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="E17" s="210">
+      <c r="E17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="F17" s="210">
+      <c r="F17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="G17" s="210">
+      <c r="G17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="H17" s="210">
+      <c r="H17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="I17" s="210">
+      <c r="I17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="J17" s="210">
+      <c r="J17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="K17" s="210">
+      <c r="K17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="L17" s="210">
+      <c r="L17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="M17" s="210">
+      <c r="M17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="N17" s="210">
+      <c r="N17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="O17" s="210">
+      <c r="O17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="P17" s="210">
+      <c r="P17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="Q17" s="210">
+      <c r="Q17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="R17" s="210">
+      <c r="R17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="S17" s="210">
+      <c r="S17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="T17" s="210">
+      <c r="T17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="U17" s="210">
+      <c r="U17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="V17" s="210">
+      <c r="V17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="W17" s="210">
+      <c r="W17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="X17" s="210">
+      <c r="X17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="Y17" s="210">
+      <c r="Y17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="Z17" s="210">
+      <c r="Z17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="AA17" s="210">
+      <c r="AA17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="AB17" s="210">
+      <c r="AB17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="AC17" s="210">
+      <c r="AC17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="AD17" s="210">
+      <c r="AD17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="AE17" s="210">
+      <c r="AE17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="AF17" s="210">
+      <c r="AF17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="AG17" s="210">
+      <c r="AG17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="AH17" s="210">
+      <c r="AH17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
-      <c r="AI17" s="210">
+      <c r="AI17" s="5">
         <f>'GREET1 Fuel_Specs'!$D$69</f>
         <v>12992301.9717196</v>
       </c>
@@ -21335,139 +21325,139 @@
       <c r="A20" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="B20" s="210">
+      <c r="B20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="C20" s="210">
+      <c r="C20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="D20" s="210">
+      <c r="D20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="E20" s="210">
+      <c r="E20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="F20" s="210">
+      <c r="F20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="G20" s="210">
+      <c r="G20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="H20" s="210">
+      <c r="H20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="I20" s="210">
+      <c r="I20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="J20" s="210">
+      <c r="J20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="K20" s="210">
+      <c r="K20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="L20" s="210">
+      <c r="L20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="M20" s="210">
+      <c r="M20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="N20" s="210">
+      <c r="N20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="O20" s="210">
+      <c r="O20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="P20" s="210">
+      <c r="P20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="Q20" s="210">
+      <c r="Q20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="R20" s="210">
+      <c r="R20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="S20" s="210">
+      <c r="S20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="T20" s="210">
+      <c r="T20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="U20" s="210">
+      <c r="U20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="V20" s="210">
+      <c r="V20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="W20" s="210">
+      <c r="W20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="X20" s="210">
+      <c r="X20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="Y20" s="210">
+      <c r="Y20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="Z20" s="210">
+      <c r="Z20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="AA20" s="210">
+      <c r="AA20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="AB20" s="210">
+      <c r="AB20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="AC20" s="210">
+      <c r="AC20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="AD20" s="210">
+      <c r="AD20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="AE20" s="210">
+      <c r="AE20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="AF20" s="210">
+      <c r="AF20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="AG20" s="210">
+      <c r="AG20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="AH20" s="210">
+      <c r="AH20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
-      <c r="AI20" s="210">
+      <c r="AI20" s="5">
         <f>'GREET1 Fuel_Specs'!$D$36</f>
         <v>91410</v>
       </c>
@@ -21766,9 +21756,7 @@
   </sheetPr>
   <dimension ref="A1:AI11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -23067,9 +23055,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Fix data error for hydrogen BTU conversion factor
</commit_message>
<xml_diff>
--- a/InputData/web-app/BCF/BTU Conversion Factors.xlsx
+++ b/InputData/web-app/BCF/BTU Conversion Factors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\web-app\BCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\web-app\BCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="gal_per_barrel">About!$A$63</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -4270,37 +4270,37 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="1" max="1" width="37.3984375" customWidth="1"/>
+    <col min="2" max="2" width="30.59765625" customWidth="1"/>
+    <col min="3" max="3" width="39.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -4309,141 +4309,141 @@
       </c>
       <c r="C6" s="202"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B8" s="3">
         <v>2019</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B10" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B13" s="196" t="s">
         <v>403</v>
       </c>
       <c r="C13" s="202"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B15" s="3">
         <v>2019</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="198" t="s">
         <v>331</v>
       </c>
       <c r="B37" s="199"/>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A38" s="203" t="s">
         <v>350</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A39" s="201" t="s">
         <v>394</v>
       </c>
@@ -4462,7 +4462,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A40" s="197" t="s">
         <v>324</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A41" s="197" t="s">
         <v>367</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A42" s="201" t="s">
         <v>388</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A43" s="201" t="s">
         <v>391</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A44" s="201" t="s">
         <v>357</v>
       </c>
@@ -4505,16 +4505,16 @@
         <v>361</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A45" s="201"/>
     </row>
-    <row r="46" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A46" s="198" t="s">
         <v>337</v>
       </c>
       <c r="B46" s="199"/>
     </row>
-    <row r="47" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A47" s="203" t="s">
         <v>350</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A48" s="201" t="s">
         <v>394</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="49" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A49" s="197" t="s">
         <v>324</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="50" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A50" s="197" t="s">
         <v>367</v>
       </c>
@@ -4546,7 +4546,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="51" spans="1:2" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A51" s="201" t="s">
         <v>393</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="52" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A52" s="201" t="s">
         <v>389</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="53" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A53" s="201" t="s">
         <v>355</v>
       </c>
@@ -4570,37 +4570,37 @@
         <v>356</v>
       </c>
     </row>
-    <row r="54" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="55" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A55" s="198" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="56" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="57" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="58" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A58" s="198" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="59" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="60" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="61" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="62" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A62" s="196" t="s">
         <v>316</v>
       </c>
       <c r="B62" s="202"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A63" s="200">
         <v>42</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A64">
         <f>3.142*10^6</f>
         <v>3142000</v>
@@ -4635,14 +4635,14 @@
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="7" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="7" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="20.86328125" style="7" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="45.73046875" style="7" customWidth="1"/>
+    <col min="3" max="16384" width="9.1328125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="18" t="s">
         <v>387</v>
       </c>
@@ -4749,8 +4749,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="20" t="s">
         <v>121</v>
       </c>
@@ -4761,7 +4761,7 @@
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
     </row>
-    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C4" s="20" t="s">
         <v>120</v>
       </c>
@@ -4774,7 +4774,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C5" s="20" t="s">
         <v>118</v>
       </c>
@@ -4785,7 +4785,7 @@
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
     </row>
-    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="20" t="s">
         <v>117</v>
       </c>
@@ -4796,7 +4796,7 @@
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
     </row>
-    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="9" t="s">
         <v>116</v>
       </c>
@@ -4804,12 +4804,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="18" t="s">
         <v>2</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="16" t="s">
         <v>2</v>
       </c>
@@ -5029,17 +5029,17 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B14" s="13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>114</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>113</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>112</v>
       </c>
@@ -5378,7 +5378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>111</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>110</v>
       </c>
@@ -5604,7 +5604,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>109</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>108</v>
       </c>
@@ -5830,7 +5830,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>107</v>
       </c>
@@ -5943,7 +5943,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>106</v>
       </c>
@@ -6056,7 +6056,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>105</v>
       </c>
@@ -6169,7 +6169,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>104</v>
       </c>
@@ -6282,7 +6282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>103</v>
       </c>
@@ -6395,7 +6395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>102</v>
       </c>
@@ -6508,7 +6508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>100</v>
       </c>
@@ -6621,7 +6621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>99</v>
       </c>
@@ -6734,7 +6734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>98</v>
       </c>
@@ -6847,7 +6847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>97</v>
       </c>
@@ -6960,7 +6960,7 @@
         <v>-2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>96</v>
       </c>
@@ -7073,7 +7073,7 @@
         <v>-2.1599999999999999E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>95</v>
       </c>
@@ -7186,7 +7186,7 @@
         <v>-2.2499999999999999E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>380</v>
       </c>
@@ -7299,7 +7299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>378</v>
       </c>
@@ -7412,7 +7412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>94</v>
       </c>
@@ -7525,7 +7525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>93</v>
       </c>
@@ -7638,7 +7638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>92</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>91</v>
       </c>
@@ -7864,7 +7864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>90</v>
       </c>
@@ -7977,7 +7977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="9" t="s">
         <v>89</v>
       </c>
@@ -8090,7 +8090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="9" t="s">
         <v>88</v>
       </c>
@@ -8203,7 +8203,7 @@
         <v>1.9699999999999999E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="9" t="s">
         <v>87</v>
       </c>
@@ -8316,7 +8316,7 @@
         <v>-4.8299999999999998E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="9" t="s">
         <v>86</v>
       </c>
@@ -8429,7 +8429,7 @@
         <v>-3.1150000000000001E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="9" t="s">
         <v>85</v>
       </c>
@@ -8542,12 +8542,12 @@
         <v>-1.013E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B47" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="9" t="s">
         <v>84</v>
       </c>
@@ -8660,7 +8660,7 @@
         <v>-2.4000000000000001E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="9" t="s">
         <v>83</v>
       </c>
@@ -8773,7 +8773,7 @@
         <v>-3.0000000000000001E-6</v>
       </c>
     </row>
-    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="9" t="s">
         <v>82</v>
       </c>
@@ -8886,7 +8886,7 @@
         <v>2.3E-5</v>
       </c>
     </row>
-    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="9" t="s">
         <v>81</v>
       </c>
@@ -8999,12 +8999,12 @@
         <v>-2.7700000000000001E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B53" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="9" t="s">
         <v>80</v>
       </c>
@@ -9117,7 +9117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
         <v>79</v>
       </c>
@@ -9230,7 +9230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="9" t="s">
         <v>78</v>
       </c>
@@ -9343,7 +9343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="9" t="s">
         <v>77</v>
       </c>
@@ -9456,7 +9456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
         <v>76</v>
       </c>
@@ -9569,7 +9569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="9" t="s">
         <v>75</v>
       </c>
@@ -9682,7 +9682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="9" t="s">
         <v>74</v>
       </c>
@@ -9795,12 +9795,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B62" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="9" t="s">
         <v>73</v>
       </c>
@@ -9913,7 +9913,7 @@
         <v>-1.4100000000000001E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="9" t="s">
         <v>72</v>
       </c>
@@ -10026,7 +10026,7 @@
         <v>-1.0139999999999999E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="9" t="s">
         <v>71</v>
       </c>
@@ -10139,7 +10139,7 @@
         <v>-2.1699999999999999E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="9" t="s">
         <v>70</v>
       </c>
@@ -10252,7 +10252,7 @@
         <v>2.8499999999999999E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="9" t="s">
         <v>69</v>
       </c>
@@ -10365,7 +10365,7 @@
         <v>2.3E-5</v>
       </c>
     </row>
-    <row r="68" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="9" t="s">
         <v>68</v>
       </c>
@@ -10478,7 +10478,7 @@
         <v>-5.5000000000000002E-5</v>
       </c>
     </row>
-    <row r="69" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="9" t="s">
         <v>67</v>
       </c>
@@ -10591,7 +10591,7 @@
         <v>-9.5000000000000005E-5</v>
       </c>
     </row>
-    <row r="70" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="9" t="s">
         <v>66</v>
       </c>
@@ -10704,7 +10704,7 @@
         <v>2.5799999999999998E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="9" t="s">
         <v>65</v>
       </c>
@@ -10817,7 +10817,7 @@
         <v>5.7700000000000004E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="9" t="s">
         <v>64</v>
       </c>
@@ -10930,7 +10930,7 @@
         <v>-1.2830000000000001E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="9" t="s">
         <v>63</v>
       </c>
@@ -11043,7 +11043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="9" t="s">
         <v>62</v>
       </c>
@@ -11156,7 +11156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
         <v>61</v>
       </c>
@@ -11269,8 +11269,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B78" s="208" t="s">
         <v>57</v>
       </c>
@@ -11310,37 +11310,37 @@
       <c r="AJ78" s="208"/>
       <c r="AK78" s="208"/>
     </row>
-    <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B79" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="80" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B80" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B81" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B82" s="8" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="83" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B83" s="8" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="84" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B84" s="8" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="85" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B85" s="8" t="s">
         <v>373</v>
       </c>
@@ -11360,40 +11360,40 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="33.140625" style="22" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="22"/>
-    <col min="11" max="11" width="10.42578125" style="22" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" style="22"/>
-    <col min="15" max="15" width="12.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="9.140625" style="22"/>
-    <col min="19" max="19" width="10.42578125" style="22" customWidth="1"/>
-    <col min="20" max="22" width="9.140625" style="22"/>
-    <col min="23" max="23" width="10.7109375" style="22" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="1" width="33.1328125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="13.3984375" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.59765625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="12.86328125" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.3984375" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.265625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" style="22" customWidth="1"/>
+    <col min="8" max="8" width="12.73046875" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.73046875" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1328125" style="22"/>
+    <col min="11" max="11" width="10.3984375" style="22" customWidth="1"/>
+    <col min="12" max="12" width="12.3984375" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.1328125" style="22"/>
+    <col min="15" max="15" width="12.86328125" style="22" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="9.1328125" style="22"/>
+    <col min="19" max="19" width="10.3984375" style="22" customWidth="1"/>
+    <col min="20" max="22" width="9.1328125" style="22"/>
+    <col min="23" max="23" width="10.73046875" style="22" customWidth="1"/>
+    <col min="24" max="16384" width="9.1328125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A1" s="21" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A2" s="23" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="24" t="s">
         <v>126</v>
       </c>
@@ -11416,7 +11416,7 @@
       </c>
       <c r="I3" s="29"/>
     </row>
-    <row r="4" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="26.65" x14ac:dyDescent="0.45">
       <c r="A4" s="30"/>
       <c r="B4" s="31" t="s">
         <v>302</v>
@@ -11441,7 +11441,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A5" s="35" t="s">
         <v>137</v>
       </c>
@@ -11458,7 +11458,7 @@
       <c r="H5" s="39"/>
       <c r="I5" s="40"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A6" s="41" t="s">
         <v>139</v>
       </c>
@@ -11483,7 +11483,7 @@
       <c r="T6" s="47"/>
       <c r="V6" s="47"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A7" s="48" t="s">
         <v>142</v>
       </c>
@@ -11520,7 +11520,7 @@
       <c r="V7" s="55"/>
       <c r="W7" s="55"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A8" s="48" t="s">
         <v>143</v>
       </c>
@@ -11557,7 +11557,7 @@
       <c r="V8" s="55"/>
       <c r="W8" s="55"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A9" s="48" t="s">
         <v>144</v>
       </c>
@@ -11594,7 +11594,7 @@
       <c r="V9" s="55"/>
       <c r="W9" s="55"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A10" s="48" t="s">
         <v>145</v>
       </c>
@@ -11627,7 +11627,7 @@
       <c r="V10" s="55"/>
       <c r="W10" s="55"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A11" s="48" t="s">
         <v>146</v>
       </c>
@@ -11668,7 +11668,7 @@
       <c r="V11" s="55"/>
       <c r="W11" s="55"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A12" s="48" t="s">
         <v>147</v>
       </c>
@@ -11705,7 +11705,7 @@
       <c r="R12" s="55"/>
       <c r="S12" s="55"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A13" s="22" t="s">
         <v>148</v>
       </c>
@@ -11734,7 +11734,7 @@
         <v>0.93726057101554028</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A14" s="22" t="s">
         <v>149</v>
       </c>
@@ -11763,7 +11763,7 @@
         <v>0.93726057101554017</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A15" s="48" t="s">
         <v>150</v>
       </c>
@@ -11801,7 +11801,7 @@
       <c r="V15" s="65"/>
       <c r="W15" s="61"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A16" s="48" t="s">
         <v>151</v>
       </c>
@@ -11835,7 +11835,7 @@
       <c r="V16" s="65"/>
       <c r="W16" s="61"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A17" s="48" t="s">
         <v>152</v>
       </c>
@@ -11873,7 +11873,7 @@
       <c r="V17" s="65"/>
       <c r="W17" s="61"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A18" s="48" t="s">
         <v>153</v>
       </c>
@@ -11907,7 +11907,7 @@
       <c r="V18" s="65"/>
       <c r="W18" s="61"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A19" s="48" t="s">
         <v>154</v>
       </c>
@@ -11941,7 +11941,7 @@
       <c r="M19" s="65"/>
       <c r="N19" s="61"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A20" s="67" t="s">
         <v>303</v>
       </c>
@@ -11972,7 +11972,7 @@
       <c r="O20" s="55"/>
       <c r="W20" s="61"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A21" s="68" t="s">
         <v>408</v>
       </c>
@@ -11999,7 +11999,7 @@
       </c>
       <c r="I21" s="54"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A22" s="48" t="s">
         <v>155</v>
       </c>
@@ -12028,7 +12028,7 @@
         <v>0.93499781627602274</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A23" s="48" t="s">
         <v>156</v>
       </c>
@@ -12057,7 +12057,7 @@
         <v>0.93499781627602274</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A24" s="48" t="s">
         <v>157</v>
       </c>
@@ -12086,7 +12086,7 @@
         <v>0.93476175247841387</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A25" s="70" t="s">
         <v>409</v>
       </c>
@@ -12115,7 +12115,7 @@
         <v>0.93404711473172097</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A26" s="71" t="s">
         <v>158</v>
       </c>
@@ -12144,7 +12144,7 @@
         <v>0.93500003751584637</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A27" s="71" t="s">
         <v>159</v>
       </c>
@@ -12173,7 +12173,7 @@
         <v>0.93500003751584626</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A28" s="71" t="s">
         <v>160</v>
       </c>
@@ -12203,7 +12203,7 @@
       </c>
       <c r="J28" s="73"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A29" s="71" t="s">
         <v>161</v>
       </c>
@@ -12232,7 +12232,7 @@
         <v>0.93499781627602263</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A30" s="71" t="s">
         <v>162</v>
       </c>
@@ -12261,7 +12261,7 @@
         <v>0.93499781627602263</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A31" s="71" t="s">
         <v>163</v>
       </c>
@@ -12291,7 +12291,7 @@
       </c>
       <c r="J31" s="73"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A32" s="71" t="s">
         <v>164</v>
       </c>
@@ -12320,7 +12320,7 @@
         <v>0.90299302022950434</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="71" t="s">
         <v>165</v>
       </c>
@@ -12350,7 +12350,7 @@
       </c>
       <c r="J33" s="73"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="71" t="s">
         <v>166</v>
       </c>
@@ -12379,7 +12379,7 @@
         <v>0.92867915675168411</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="71" t="s">
         <v>167</v>
       </c>
@@ -12409,7 +12409,7 @@
       </c>
       <c r="J35" s="73"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="71" t="s">
         <v>168</v>
       </c>
@@ -12439,7 +12439,7 @@
       </c>
       <c r="J36" s="73"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="71" t="s">
         <v>169</v>
       </c>
@@ -12469,7 +12469,7 @@
       </c>
       <c r="J37" s="73"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="71" t="s">
         <v>170</v>
       </c>
@@ -12499,7 +12499,7 @@
       </c>
       <c r="J38" s="73"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="71" t="s">
         <v>171</v>
       </c>
@@ -12530,7 +12530,7 @@
       <c r="J39" s="73"/>
       <c r="K39" s="73"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="71" t="s">
         <v>172</v>
       </c>
@@ -12561,7 +12561,7 @@
       <c r="J40" s="73"/>
       <c r="K40" s="73"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="71" t="s">
         <v>173</v>
       </c>
@@ -12591,7 +12591,7 @@
       </c>
       <c r="K41" s="73"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="70" t="s">
         <v>174</v>
       </c>
@@ -12621,7 +12621,7 @@
       </c>
       <c r="K42" s="73"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="70" t="s">
         <v>175</v>
       </c>
@@ -12651,7 +12651,7 @@
       </c>
       <c r="K43" s="73"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" s="71" t="s">
         <v>176</v>
       </c>
@@ -12681,7 +12681,7 @@
       </c>
       <c r="K44" s="73"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" s="22" t="s">
         <v>177</v>
       </c>
@@ -12710,7 +12710,7 @@
         <v>0.93361506882395562</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" s="71" t="s">
         <v>178</v>
       </c>
@@ -12740,7 +12740,7 @@
       </c>
       <c r="K46" s="73"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" s="48" t="s">
         <v>410</v>
       </c>
@@ -12769,7 +12769,7 @@
         <v>0.93361506882395551</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="48" t="s">
         <v>179</v>
       </c>
@@ -12798,7 +12798,7 @@
         <v>0.93500003751584626</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A49" s="48" t="s">
         <v>180</v>
       </c>
@@ -12828,7 +12828,7 @@
       </c>
       <c r="J49" s="73"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A50" s="48" t="s">
         <v>181</v>
       </c>
@@ -12858,7 +12858,7 @@
       </c>
       <c r="J50" s="73"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A51" s="48" t="s">
         <v>182</v>
       </c>
@@ -12888,7 +12888,7 @@
       </c>
       <c r="J51" s="73"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A52" s="48" t="s">
         <v>183</v>
       </c>
@@ -12918,7 +12918,7 @@
       </c>
       <c r="J52" s="73"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A53" s="48" t="s">
         <v>184</v>
       </c>
@@ -12948,7 +12948,7 @@
       </c>
       <c r="J53" s="73"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A54" s="48" t="s">
         <v>185</v>
       </c>
@@ -12978,7 +12978,7 @@
       </c>
       <c r="J54" s="73"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A55" s="48" t="s">
         <v>186</v>
       </c>
@@ -13008,7 +13008,7 @@
       </c>
       <c r="J55" s="73"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A56" s="67" t="s">
         <v>187</v>
       </c>
@@ -13037,7 +13037,7 @@
         <v>0.92157077225989936</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A57" s="48" t="s">
         <v>188</v>
       </c>
@@ -13064,7 +13064,7 @@
         <v>0.92932939503336609</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A58" s="41" t="s">
         <v>189</v>
       </c>
@@ -13093,7 +13093,7 @@
         <v>0.93722267739953979</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A59" s="48" t="s">
         <v>191</v>
       </c>
@@ -13116,7 +13116,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A60" s="67" t="s">
         <v>194</v>
       </c>
@@ -13145,7 +13145,7 @@
         <v>0.90266299357208446</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A61" s="48" t="s">
         <v>195</v>
       </c>
@@ -13175,7 +13175,7 @@
       </c>
       <c r="L61" s="47"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A62" s="48" t="s">
         <v>196</v>
       </c>
@@ -13204,7 +13204,7 @@
         <v>0.84548104956268222</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A63" s="71" t="s">
         <v>197</v>
       </c>
@@ -13225,7 +13225,7 @@
       </c>
       <c r="I63" s="54"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A64" s="41" t="s">
         <v>190</v>
       </c>
@@ -13255,7 +13255,7 @@
       </c>
       <c r="K64" s="47"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A65" s="67" t="s">
         <v>198</v>
       </c>
@@ -13276,7 +13276,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A66" s="68" t="s">
         <v>200</v>
       </c>
@@ -13302,7 +13302,7 @@
       <c r="I66" s="94"/>
       <c r="K66" s="95"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A67" s="68" t="s">
         <v>201</v>
       </c>
@@ -13330,7 +13330,7 @@
       </c>
       <c r="K67" s="95"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A68" s="68" t="s">
         <v>202</v>
       </c>
@@ -13358,7 +13358,7 @@
       </c>
       <c r="K68" s="95"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A69" s="68" t="s">
         <v>203</v>
       </c>
@@ -13386,7 +13386,7 @@
       </c>
       <c r="K69" s="95"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A70" s="68" t="s">
         <v>204</v>
       </c>
@@ -13415,7 +13415,7 @@
       <c r="K70" s="95"/>
       <c r="M70" s="73"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A71" s="71" t="s">
         <v>205</v>
       </c>
@@ -13444,7 +13444,7 @@
       <c r="K71" s="95"/>
       <c r="L71" s="95"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A72" s="70" t="s">
         <v>206</v>
       </c>
@@ -13472,7 +13472,7 @@
       </c>
       <c r="K72" s="95"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A73" s="48" t="s">
         <v>207</v>
       </c>
@@ -13499,7 +13499,7 @@
         <v>0.94242199100000001</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="12.6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="48" t="s">
         <v>208</v>
       </c>
@@ -13527,7 +13527,7 @@
       </c>
       <c r="K74" s="97"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A75" s="48" t="s">
         <v>411</v>
       </c>
@@ -13555,7 +13555,7 @@
       </c>
       <c r="K75" s="97"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A76" s="48" t="s">
         <v>209</v>
       </c>
@@ -13582,7 +13582,7 @@
         <v>0.93173565722585328</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A77" s="70" t="s">
         <v>210</v>
       </c>
@@ -13611,7 +13611,7 @@
       <c r="J77" s="55"/>
       <c r="K77" s="98"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A78" s="71" t="s">
         <v>211</v>
       </c>
@@ -13639,7 +13639,7 @@
       </c>
       <c r="K78" s="97"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A79" s="71" t="s">
         <v>212</v>
       </c>
@@ -13666,7 +13666,7 @@
         <v>0.93680161201685286</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A80" s="71" t="s">
         <v>213</v>
       </c>
@@ -13693,7 +13693,7 @@
         <v>0.93292760238366934</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A81" s="71" t="s">
         <v>214</v>
       </c>
@@ -13720,7 +13720,7 @@
         <v>0.96554227633195577</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A82" s="71" t="s">
         <v>412</v>
       </c>
@@ -13747,7 +13747,7 @@
         <v>0.93359512366662756</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A83" s="99" t="s">
         <v>215</v>
       </c>
@@ -13770,7 +13770,7 @@
       </c>
       <c r="I83" s="102"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A84" s="103" t="s">
         <v>216</v>
       </c>
@@ -13793,7 +13793,7 @@
         <v>0.85292563033160751</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A85" s="103" t="s">
         <v>217</v>
       </c>
@@ -13816,7 +13816,7 @@
         <v>0.88047037071579148</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A86" s="103" t="s">
         <v>218</v>
       </c>
@@ -13843,7 +13843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A87" s="106" t="s">
         <v>219</v>
       </c>
@@ -13870,7 +13870,7 @@
         <v>0.90447216306662592</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A88" s="107" t="s">
         <v>220</v>
       </c>
@@ -13897,7 +13897,7 @@
         <v>0.94150280898876404</v>
       </c>
     </row>
-    <row r="89" spans="1:14" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" s="73" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A89" s="73" t="s">
         <v>221</v>
       </c>
@@ -13924,7 +13924,7 @@
         <v>0.94150280898876404</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A90" s="23" t="s">
         <v>222</v>
       </c>
@@ -13951,7 +13951,7 @@
         <v>0.8252427184466018</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A91" s="73" t="s">
         <v>223</v>
       </c>
@@ -13978,7 +13978,7 @@
         <v>0.87681159420289856</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A92" s="118" t="s">
         <v>413</v>
       </c>
@@ -14012,7 +14012,7 @@
       <c r="M92" s="121"/>
       <c r="N92" s="122"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A93" s="123" t="s">
         <v>414</v>
       </c>
@@ -14038,12 +14038,12 @@
       <c r="M93" s="125"/>
       <c r="N93" s="126"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A94" s="127"/>
       <c r="B94" s="128"/>
       <c r="N94" s="129"/>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A95" s="127" t="s">
         <v>224</v>
       </c>
@@ -14058,7 +14058,7 @@
       <c r="M95" s="73"/>
       <c r="N95" s="129"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A96" s="130" t="s">
         <v>225</v>
       </c>
@@ -14076,7 +14076,7 @@
       <c r="M96" s="133"/>
       <c r="N96" s="134"/>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A97" s="135" t="s">
         <v>226</v>
       </c>
@@ -14120,7 +14120,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A98" s="136" t="s">
         <v>233</v>
       </c>
@@ -14164,7 +14164,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A99" s="137" t="s">
         <v>234</v>
       </c>
@@ -14208,7 +14208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A100" s="123" t="s">
         <v>235</v>
       </c>
@@ -14252,7 +14252,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A101" s="127" t="s">
         <v>236</v>
       </c>
@@ -14296,13 +14296,13 @@
         <v>270</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A102" s="127"/>
       <c r="B102" s="128"/>
       <c r="F102" s="73"/>
       <c r="G102" s="129"/>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A103" s="127" t="s">
         <v>237</v>
       </c>
@@ -14311,7 +14311,7 @@
       <c r="F103" s="73"/>
       <c r="G103" s="129"/>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A104" s="127" t="s">
         <v>238</v>
       </c>
@@ -14334,7 +14334,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A105" s="130" t="s">
         <v>233</v>
       </c>
@@ -14355,7 +14355,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A106" s="22" t="s">
         <v>242</v>
       </c>
@@ -14378,7 +14378,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A107" s="23" t="s">
         <v>243</v>
       </c>
@@ -14401,7 +14401,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A108" s="118" t="s">
         <v>244</v>
       </c>
@@ -14424,7 +14424,7 @@
         <v>-87</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A109" s="127" t="s">
         <v>245</v>
       </c>
@@ -14447,7 +14447,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A110" s="127" t="s">
         <v>246</v>
       </c>
@@ -14470,17 +14470,17 @@
         <v>-71</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A111" s="127"/>
       <c r="B111" s="146"/>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A112" s="130" t="s">
         <v>247</v>
       </c>
       <c r="B112" s="147"/>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A113" s="22" t="s">
         <v>248</v>
       </c>
@@ -14488,7 +14488,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A114" s="148" t="s">
         <v>249</v>
       </c>
@@ -14498,7 +14498,7 @@
       <c r="C114" s="73"/>
       <c r="D114" s="73"/>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A115" s="73" t="s">
         <v>250</v>
       </c>
@@ -14506,7 +14506,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A116" s="22" t="s">
         <v>251</v>
       </c>
@@ -14519,7 +14519,7 @@
       <c r="R116" s="151"/>
       <c r="V116" s="151"/>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A117" s="22" t="s">
         <v>252</v>
       </c>
@@ -14532,7 +14532,7 @@
       <c r="R117" s="154"/>
       <c r="V117" s="154"/>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.45">
       <c r="B118" s="155"/>
       <c r="C118" s="156"/>
       <c r="D118" s="157"/>
@@ -14552,7 +14552,7 @@
       <c r="W118" s="158"/>
       <c r="X118" s="157"/>
     </row>
-    <row r="119" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A119" s="73" t="s">
         <v>253</v>
       </c>
@@ -14575,7 +14575,7 @@
       <c r="W119" s="160"/>
       <c r="X119" s="161"/>
     </row>
-    <row r="120" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B120" s="162"/>
       <c r="C120" s="163"/>
       <c r="D120" s="164"/>
@@ -14595,7 +14595,7 @@
       <c r="W120" s="163"/>
       <c r="X120" s="164"/>
     </row>
-    <row r="121" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B121" s="162">
         <v>10</v>
       </c>
@@ -14627,7 +14627,7 @@
       <c r="W121" s="163"/>
       <c r="X121" s="164"/>
     </row>
-    <row r="122" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B122" s="162">
         <v>10</v>
       </c>
@@ -14659,7 +14659,7 @@
       <c r="W122" s="163"/>
       <c r="X122" s="164"/>
     </row>
-    <row r="123" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B123" s="162" t="s">
         <v>254</v>
       </c>
@@ -14715,7 +14715,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="124" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B124" s="162">
         <v>1990</v>
       </c>
@@ -14771,7 +14771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:24" s="73" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B125" s="162">
         <v>1995</v>
       </c>
@@ -14827,7 +14827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:24" x14ac:dyDescent="0.45">
       <c r="B126" s="168">
         <v>2000</v>
       </c>
@@ -14883,7 +14883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:24" x14ac:dyDescent="0.45">
       <c r="B127" s="22">
         <v>2005</v>
       </c>
@@ -14939,7 +14939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A128" s="148"/>
       <c r="B128" s="22">
         <v>2010</v>
@@ -14996,7 +14996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A129" s="171"/>
       <c r="B129" s="172">
         <v>2015</v>
@@ -15054,7 +15054,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A130" s="175"/>
       <c r="B130" s="176">
         <v>2017</v>
@@ -15112,7 +15112,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="131" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A131" s="175"/>
       <c r="B131" s="179">
         <v>2020</v>
@@ -15128,7 +15128,7 @@
       <c r="G131" s="174"/>
       <c r="H131" s="174"/>
     </row>
-    <row r="132" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A132" s="175"/>
       <c r="B132" s="179"/>
       <c r="C132" s="179"/>
@@ -15138,7 +15138,7 @@
       <c r="G132" s="174"/>
       <c r="H132" s="174"/>
     </row>
-    <row r="133" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A133" s="175" t="s">
         <v>262</v>
       </c>
@@ -15150,7 +15150,7 @@
       <c r="G133" s="174"/>
       <c r="H133" s="174"/>
     </row>
-    <row r="134" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A134" s="181" t="s">
         <v>263</v>
       </c>
@@ -15172,7 +15172,7 @@
       <c r="G134" s="174"/>
       <c r="H134" s="174"/>
     </row>
-    <row r="135" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A135" s="174" t="s">
         <v>269</v>
       </c>
@@ -15194,7 +15194,7 @@
       <c r="G135" s="174"/>
       <c r="H135" s="174"/>
     </row>
-    <row r="136" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A136" s="171" t="s">
         <v>270</v>
       </c>
@@ -15216,7 +15216,7 @@
       <c r="G136" s="174"/>
       <c r="H136" s="174"/>
     </row>
-    <row r="137" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A137" s="175" t="s">
         <v>271</v>
       </c>
@@ -15238,7 +15238,7 @@
       <c r="G137" s="174"/>
       <c r="H137" s="174"/>
     </row>
-    <row r="138" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A138" s="175" t="s">
         <v>272</v>
       </c>
@@ -15260,7 +15260,7 @@
       <c r="G138" s="174"/>
       <c r="H138" s="174"/>
     </row>
-    <row r="139" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A139" s="175" t="s">
         <v>273</v>
       </c>
@@ -15282,7 +15282,7 @@
       <c r="G139" s="174"/>
       <c r="H139" s="174"/>
     </row>
-    <row r="140" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A140" s="175"/>
       <c r="B140" s="163"/>
       <c r="C140" s="179"/>
@@ -15292,7 +15292,7 @@
       <c r="G140" s="174"/>
       <c r="H140" s="174"/>
     </row>
-    <row r="141" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A141" s="181" t="s">
         <v>274</v>
       </c>
@@ -15314,7 +15314,7 @@
       <c r="G141" s="174"/>
       <c r="H141" s="174"/>
     </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A142" s="174" t="s">
         <v>280</v>
       </c>
@@ -15336,7 +15336,7 @@
       <c r="G142" s="174"/>
       <c r="H142" s="174"/>
     </row>
-    <row r="143" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A143" s="171" t="s">
         <v>281</v>
       </c>
@@ -15359,7 +15359,7 @@
       <c r="H143" s="172"/>
       <c r="I143" s="190"/>
     </row>
-    <row r="144" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A144" s="175" t="s">
         <v>282</v>
       </c>
@@ -15382,7 +15382,7 @@
       <c r="H144" s="176"/>
       <c r="I144" s="129"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A145" s="175" t="s">
         <v>283</v>
       </c>
@@ -15405,7 +15405,7 @@
       <c r="H145" s="176"/>
       <c r="I145" s="129"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A146" s="175" t="s">
         <v>284</v>
       </c>
@@ -15428,7 +15428,7 @@
       <c r="H146" s="176"/>
       <c r="I146" s="129"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A147" s="175"/>
       <c r="B147" s="179"/>
       <c r="C147" s="177"/>
@@ -15439,7 +15439,7 @@
       <c r="H147" s="176"/>
       <c r="I147" s="129"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A148" s="175" t="s">
         <v>285</v>
       </c>
@@ -15468,7 +15468,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A149" s="175" t="s">
         <v>294</v>
       </c>
@@ -15497,7 +15497,7 @@
         <v>2684519.5376862194</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A150" s="175" t="s">
         <v>295</v>
       </c>
@@ -15526,7 +15526,7 @@
         <v>2684.5195376862198</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A151" s="195" t="s">
         <v>296</v>
       </c>
@@ -15555,7 +15555,7 @@
         <v>2.6845195376862194</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A152" s="22" t="s">
         <v>297</v>
       </c>
@@ -15584,7 +15584,7 @@
         <v>745.69987157950538</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A153" s="22" t="s">
         <v>298</v>
       </c>
@@ -15613,7 +15613,7 @@
         <v>0.74569987157950535</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A154" s="22" t="s">
         <v>299</v>
       </c>
@@ -15642,7 +15642,7 @@
         <v>2544.4335839531336</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A155" s="22" t="s">
         <v>300</v>
       </c>
@@ -15671,7 +15671,7 @@
         <v>2.5444335839531337E-3</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A156" s="22" t="s">
         <v>301</v>
       </c>
@@ -15700,7 +15700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A158" s="22" t="s">
         <v>415</v>
       </c>
@@ -15720,7 +15720,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A159" s="22" t="s">
         <v>416</v>
       </c>
@@ -15740,7 +15740,7 @@
         <v>1609340</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A160" s="22" t="s">
         <v>417</v>
       </c>
@@ -15760,7 +15760,7 @@
         <v>1609.34</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A161" s="22" t="s">
         <v>418</v>
       </c>
@@ -15780,7 +15780,7 @@
         <v>1.60934</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A162" s="22" t="s">
         <v>419</v>
       </c>
@@ -15800,7 +15800,7 @@
         <v>5280</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A163" s="22" t="s">
         <v>420</v>
       </c>
@@ -15850,16 +15850,18 @@
   </sheetPr>
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="U13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:AI22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.86328125" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="35" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>407</v>
       </c>
@@ -15966,7 +15968,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>347</v>
       </c>
@@ -16107,7 +16109,7 @@
         <v>3142000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>323</v>
       </c>
@@ -16248,7 +16250,7 @@
         <v>19887484000000</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>324</v>
       </c>
@@ -16389,7 +16391,7 @@
         <v>1036999999999999.9</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>341</v>
       </c>
@@ -16530,7 +16532,7 @@
         <v>1000000000000</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>342</v>
       </c>
@@ -16637,7 +16639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>343</v>
       </c>
@@ -16744,7 +16746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>344</v>
       </c>
@@ -16851,7 +16853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>325</v>
       </c>
@@ -16992,7 +16994,7 @@
         <v>17906000000000</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>326</v>
       </c>
@@ -17133,7 +17135,7 @@
         <v>5023036000000</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>327</v>
       </c>
@@ -17274,7 +17276,7 @@
         <v>5825000000000</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>328</v>
       </c>
@@ -17415,7 +17417,7 @@
         <v>3989233000000</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>329</v>
       </c>
@@ -17556,7 +17558,7 @@
         <v>5359000000000</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>372</v>
       </c>
@@ -17697,7 +17699,7 @@
         <v>5670000000000</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>348</v>
       </c>
@@ -17838,7 +17840,7 @@
         <v>3142000000000</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>345</v>
       </c>
@@ -17945,7 +17947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>330</v>
       </c>
@@ -18086,7 +18088,7 @@
         <v>12992301971719.6</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>368</v>
       </c>
@@ -18227,7 +18229,7 @@
         <v>5676202000000</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>369</v>
       </c>
@@ -18368,7 +18370,7 @@
         <v>6287000000000</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>370</v>
       </c>
@@ -18509,7 +18511,7 @@
         <v>91410000000</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>371</v>
       </c>
@@ -18650,145 +18652,145 @@
         <v>13583444584264.561</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>367</v>
       </c>
       <c r="B22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="C22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="D22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="E22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="F22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="G22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="H22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="I22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="J22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="K22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="L22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="M22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="N22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="O22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="P22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="Q22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="R22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="S22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="T22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="U22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="V22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="W22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="X22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="Y22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="Z22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AA22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AB22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AC22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AD22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AE22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AF22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AG22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AH22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
       <c r="AI22" s="207">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>874650000000</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
+        <v>134509803921.56865</v>
       </c>
     </row>
   </sheetData>
@@ -18803,16 +18805,18 @@
   </sheetPr>
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="U10" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:AI22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="30.86328125" style="2" customWidth="1"/>
     <col min="2" max="35" width="10" style="2" customWidth="1"/>
-    <col min="36" max="16384" width="9.140625" style="2"/>
+    <col min="36" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>406</v>
       </c>
@@ -18919,7 +18923,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>353</v>
       </c>
@@ -19060,7 +19064,7 @@
         <v>3142000</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>323</v>
       </c>
@@ -19201,7 +19205,7 @@
         <v>19887484</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>324</v>
       </c>
@@ -19342,7 +19346,7 @@
         <v>1036999.9999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>359</v>
       </c>
@@ -19483,7 +19487,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>342</v>
       </c>
@@ -19590,7 +19594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>343</v>
       </c>
@@ -19697,7 +19701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>344</v>
       </c>
@@ -19804,7 +19808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>325</v>
       </c>
@@ -19945,7 +19949,7 @@
         <v>17906000</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>326</v>
       </c>
@@ -20086,7 +20090,7 @@
         <v>119596.09523809524</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>327</v>
       </c>
@@ -20227,7 +20231,7 @@
         <v>138690.47619047618</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>328</v>
       </c>
@@ -20368,7 +20372,7 @@
         <v>94981.738095238092</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>329</v>
       </c>
@@ -20509,7 +20513,7 @@
         <v>127595.23809523809</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>372</v>
       </c>
@@ -20650,7 +20654,7 @@
         <v>135000</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>354</v>
       </c>
@@ -20791,7 +20795,7 @@
         <v>3142000</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>345</v>
       </c>
@@ -20898,7 +20902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>330</v>
       </c>
@@ -21039,7 +21043,7 @@
         <v>12992301.9717196</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>368</v>
       </c>
@@ -21180,7 +21184,7 @@
         <v>5676202</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>369</v>
       </c>
@@ -21321,7 +21325,7 @@
         <v>6287000</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>370</v>
       </c>
@@ -21462,7 +21466,7 @@
         <v>91410</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>371</v>
       </c>
@@ -21603,145 +21607,145 @@
         <v>13583444.58426456</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>367</v>
       </c>
       <c r="B22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="C22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="D22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="E22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="F22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="G22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="H22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="I22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="J22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="K22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="L22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="M22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="N22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="O22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="P22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="Q22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="R22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="S22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="T22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="U22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="V22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="W22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="X22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="Y22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="Z22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AA22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AB22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AC22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AD22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AE22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AF22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AG22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AH22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
       <c r="AI22" s="5">
-        <f>'GREET1 Fuel_Specs'!$D$62*'GREET1 Fuel_Specs'!$E$62*10^3</f>
-        <v>874650</v>
+        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^3</f>
+        <v>134509.80392156864</v>
       </c>
     </row>
   </sheetData>
@@ -21758,13 +21762,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="1" max="1" width="38.265625" customWidth="1"/>
     <col min="2" max="35" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>405</v>
       </c>
@@ -21871,7 +21875,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>310</v>
       </c>
@@ -21978,7 +21982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>311</v>
       </c>
@@ -22085,7 +22089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>318</v>
       </c>
@@ -22226,7 +22230,7 @@
         <v>119596.09523809524</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>319</v>
       </c>
@@ -22367,7 +22371,7 @@
         <v>138690.47619047618</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>312</v>
       </c>
@@ -22474,7 +22478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>313</v>
       </c>
@@ -22581,7 +22585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>320</v>
       </c>
@@ -22722,7 +22726,7 @@
         <v>135000</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>402</v>
       </c>
@@ -22829,7 +22833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>370</v>
       </c>
@@ -22936,7 +22940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>367</v>
       </c>
@@ -23057,14 +23061,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>299</v>
       </c>

</xml_diff>

<commit_message>
New output graph for hydrogen production + input file to convert to MMT H2
</commit_message>
<xml_diff>
--- a/InputData/web-app/BCF/BTU Conversion Factors.xlsx
+++ b/InputData/web-app/BCF/BTU Conversion Factors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\web-app\BCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B325659A-AC75-4AA0-B1D5-E255D1F9BDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F17E76-1DE8-4C0C-BDAB-6D3A2549A6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1545" yWindow="1335" windowWidth="20985" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,9 +20,10 @@
     <sheet name="BCF-BpSFOU" sheetId="12" r:id="rId5"/>
     <sheet name="BCF-VFEUCF" sheetId="10" r:id="rId6"/>
     <sheet name="BCF-BpEIEOU" sheetId="13" r:id="rId7"/>
+    <sheet name="BCF-BpMMTH" sheetId="15" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="gal_per_barrel">About!$A$66</definedName>
+    <definedName name="gal_per_barrel">About!$A$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1190,7 +1191,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="433">
   <si>
     <t>(from physical units to million Btu)</t>
   </si>
@@ -2465,6 +2466,30 @@
   </si>
   <si>
     <t>you</t>
+  </si>
+  <si>
+    <t>BCF BTU per MMT Hydrogen</t>
+  </si>
+  <si>
+    <t>Hydrogen Energy Density</t>
+  </si>
+  <si>
+    <t>DOE</t>
+  </si>
+  <si>
+    <t>Alternative Fuels Data Center Fuel Properties Comparison</t>
+  </si>
+  <si>
+    <t>https://afdc.energy.gov/files/u/publication/fuel_comparison_chart.pdf</t>
+  </si>
+  <si>
+    <t>Higher heating value energy content</t>
+  </si>
+  <si>
+    <t>btu/MMT</t>
+  </si>
+  <si>
+    <t>btu/lb H2</t>
   </si>
 </sst>
 </file>
@@ -2487,7 +2512,7 @@
     <numFmt numFmtId="175" formatCode="#,##0.0000000000"/>
     <numFmt numFmtId="176" formatCode="#,##0.0000000"/>
   </numFmts>
-  <fonts count="39" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2758,6 +2783,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="44">
@@ -3489,7 +3522,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3848,6 +3881,7 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="55">
       <alignment wrapText="1"/>
     </xf>
@@ -4247,10 +4281,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4281,326 +4315,375 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="173" t="s">
+      <c r="B7" s="173" t="s">
         <v>345</v>
       </c>
-      <c r="C6" s="177"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="C7" s="177"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="173" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="173" t="s">
         <v>401</v>
       </c>
-      <c r="C13" s="177"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="C14" s="177"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
         <v>2019</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>306</v>
+        <v>419</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="173" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>308</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="174" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="174" t="s">
         <v>331</v>
       </c>
-      <c r="B40" s="175"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>349</v>
-      </c>
-      <c r="B41" t="s">
-        <v>350</v>
-      </c>
-      <c r="C41" s="178" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="176" t="s">
-        <v>392</v>
-      </c>
-      <c r="B42" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>324</v>
-      </c>
-      <c r="B43" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>366</v>
-      </c>
-      <c r="B44" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="176" t="s">
-        <v>387</v>
-      </c>
-      <c r="B45" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="176" t="s">
-        <v>389</v>
-      </c>
-      <c r="B46" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="176" t="s">
-        <v>356</v>
-      </c>
-      <c r="B47" t="s">
-        <v>357</v>
-      </c>
-      <c r="C47" s="178" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="176"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="174" t="s">
-        <v>336</v>
-      </c>
       <c r="B49" s="175"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>349</v>
       </c>
       <c r="B50" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+      <c r="C50" s="178" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="176" t="s">
         <v>392</v>
       </c>
       <c r="B51" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>324</v>
       </c>
       <c r="B52" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>366</v>
       </c>
       <c r="B53" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="176" t="s">
+        <v>387</v>
+      </c>
+      <c r="B54" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="176" t="s">
+        <v>389</v>
+      </c>
+      <c r="B55" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="176" t="s">
+        <v>356</v>
+      </c>
+      <c r="B56" t="s">
+        <v>357</v>
+      </c>
+      <c r="C56" s="178" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="176"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="174" t="s">
+        <v>336</v>
+      </c>
+      <c r="B58" s="175"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>349</v>
+      </c>
+      <c r="B59" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="176" t="s">
+        <v>392</v>
+      </c>
+      <c r="B60" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>324</v>
+      </c>
+      <c r="B61" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>366</v>
+      </c>
+      <c r="B62" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="176" t="s">
+    <row r="63" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="176" t="s">
         <v>391</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B63" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="176" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="176" t="s">
         <v>388</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B64" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="176" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="176" t="s">
         <v>354</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B65" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="174" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="174" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="174" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="174" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="173" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="173" t="s">
         <v>316</v>
       </c>
-      <c r="B65" s="177"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66">
+      <c r="B74" s="177"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
         <v>42</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B75" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
         <f>3.41214*10^6</f>
         <v>3412140</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B76" t="s">
         <v>339</v>
       </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>61013</v>
+      </c>
+      <c r="B77" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="182"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11256,44 +11339,44 @@
     </row>
     <row r="77" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="182" t="s">
+      <c r="B78" s="183" t="s">
         <v>57</v>
       </c>
-      <c r="C78" s="182"/>
-      <c r="D78" s="182"/>
-      <c r="E78" s="182"/>
-      <c r="F78" s="182"/>
-      <c r="G78" s="182"/>
-      <c r="H78" s="182"/>
-      <c r="I78" s="182"/>
-      <c r="J78" s="182"/>
-      <c r="K78" s="182"/>
-      <c r="L78" s="182"/>
-      <c r="M78" s="182"/>
-      <c r="N78" s="182"/>
-      <c r="O78" s="182"/>
-      <c r="P78" s="182"/>
-      <c r="Q78" s="182"/>
-      <c r="R78" s="182"/>
-      <c r="S78" s="182"/>
-      <c r="T78" s="182"/>
-      <c r="U78" s="182"/>
-      <c r="V78" s="182"/>
-      <c r="W78" s="182"/>
-      <c r="X78" s="182"/>
-      <c r="Y78" s="182"/>
-      <c r="Z78" s="182"/>
-      <c r="AA78" s="182"/>
-      <c r="AB78" s="182"/>
-      <c r="AC78" s="182"/>
-      <c r="AD78" s="182"/>
-      <c r="AE78" s="182"/>
-      <c r="AF78" s="182"/>
-      <c r="AG78" s="182"/>
-      <c r="AH78" s="182"/>
-      <c r="AI78" s="182"/>
-      <c r="AJ78" s="182"/>
-      <c r="AK78" s="182"/>
+      <c r="C78" s="183"/>
+      <c r="D78" s="183"/>
+      <c r="E78" s="183"/>
+      <c r="F78" s="183"/>
+      <c r="G78" s="183"/>
+      <c r="H78" s="183"/>
+      <c r="I78" s="183"/>
+      <c r="J78" s="183"/>
+      <c r="K78" s="183"/>
+      <c r="L78" s="183"/>
+      <c r="M78" s="183"/>
+      <c r="N78" s="183"/>
+      <c r="O78" s="183"/>
+      <c r="P78" s="183"/>
+      <c r="Q78" s="183"/>
+      <c r="R78" s="183"/>
+      <c r="S78" s="183"/>
+      <c r="T78" s="183"/>
+      <c r="U78" s="183"/>
+      <c r="V78" s="183"/>
+      <c r="W78" s="183"/>
+      <c r="X78" s="183"/>
+      <c r="Y78" s="183"/>
+      <c r="Z78" s="183"/>
+      <c r="AA78" s="183"/>
+      <c r="AB78" s="183"/>
+      <c r="AC78" s="183"/>
+      <c r="AD78" s="183"/>
+      <c r="AE78" s="183"/>
+      <c r="AF78" s="183"/>
+      <c r="AG78" s="183"/>
+      <c r="AH78" s="183"/>
+      <c r="AI78" s="183"/>
+      <c r="AJ78" s="183"/>
+      <c r="AK78" s="183"/>
     </row>
     <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="6" t="s">
@@ -15842,139 +15925,139 @@
         <v>346</v>
       </c>
       <c r="B2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="C2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="D2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="E2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="F2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="G2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="H2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="I2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="J2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="K2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="L2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="M2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="N2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="O2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="P2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="Q2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="R2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="S2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="T2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="U2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="V2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="W2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="X2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="Y2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="Z2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AA2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AB2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AC2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AD2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AE2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AF2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AG2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AH2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AI2">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
     </row>
@@ -17572,139 +17655,139 @@
         <v>347</v>
       </c>
       <c r="B15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="C15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="D15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="E15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="F15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="G15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="H15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="I15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="J15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="K15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="L15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="M15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="N15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="O15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="P15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="Q15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="R15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="S15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="T15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="U15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="V15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="W15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="X15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="Y15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="Z15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AA15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AB15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AC15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AD15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AE15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AF15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AG15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AH15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
       <c r="AI15">
-        <f>About!$A$67*10^6</f>
+        <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
     </row>
@@ -18795,139 +18878,139 @@
         <v>352</v>
       </c>
       <c r="B2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="C2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="D2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="E2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="F2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="G2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="H2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="I2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="J2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="K2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="L2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="M2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="N2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="O2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="P2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="Q2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="R2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="S2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="T2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="U2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="V2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="W2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="X2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="Y2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="Z2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AA2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AB2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AC2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AD2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AE2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AF2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AG2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AH2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AI2">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
     </row>
@@ -20526,139 +20609,139 @@
         <v>353</v>
       </c>
       <c r="B15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="C15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="D15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="E15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="F15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="G15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="H15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="I15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="J15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="K15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="L15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="M15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="N15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="O15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="P15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="Q15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="R15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="S15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="T15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="U15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="V15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="W15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="X15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="Y15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="Z15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AA15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AB15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AC15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AD15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AE15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AF15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AG15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AH15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
       <c r="AI15">
-        <f>About!$A$67</f>
+        <f>About!$A$76</f>
         <v>3412140</v>
       </c>
     </row>
@@ -22928,9 +23011,14 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -22942,9 +23030,44 @@
         <v>299</v>
       </c>
       <c r="B2">
-        <f>10^12</f>
-        <v>1000000000000</v>
-      </c>
+        <f>CONVERT(About!A77,"kg","lbm")*1000000000</f>
+        <v>134510640026859.36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E207D541-9B8A-44C9-8F50-D7BD086C4684}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>CONVERT(About!A77,"kg","lbm")*1000000000</f>
+        <v>134510640026859.36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="182"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
re export BCF, take out you
</commit_message>
<xml_diff>
--- a/InputData/web-app/BCF/BTU Conversion Factors.xlsx
+++ b/InputData/web-app/BCF/BTU Conversion Factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\web-app\BCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\United States\us-eps\InputData\web-app\BCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F17E76-1DE8-4C0C-BDAB-6D3A2549A6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164845E5-F203-493C-B648-3ABC9D0083FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="1335" windowWidth="20985" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="130" yWindow="0" windowWidth="17840" windowHeight="10080" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1191,7 +1191,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="432">
   <si>
     <t>(from physical units to million Btu)</t>
   </si>
@@ -2463,9 +2463,6 @@
   </si>
   <si>
     <t>barrels of oil</t>
-  </si>
-  <si>
-    <t>you</t>
   </si>
   <si>
     <t>BCF BTU per MMT Hydrogen</t>
@@ -4283,46 +4280,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+    <sheetView topLeftCell="A60" workbookViewId="0">
       <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="1" max="1" width="37.40625" customWidth="1"/>
+    <col min="2" max="2" width="30.54296875" customWidth="1"/>
+    <col min="3" max="3" width="39.40625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -4331,177 +4328,177 @@
       </c>
       <c r="C7" s="177"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B9" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B10" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B11" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B12" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B14" s="173" t="s">
         <v>401</v>
       </c>
       <c r="C14" s="177"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B15" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B16" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B17" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B18" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B19" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B21" s="173" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B22" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B23" s="2">
         <v>2021</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B24" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B25" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B26" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A29" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A31" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A33" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A34" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A35" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A36" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A37" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A38" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A40" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A41" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A42" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A44" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A45" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A47" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A49" s="174" t="s">
         <v>331</v>
       </c>
       <c r="B49" s="175"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A50" t="s">
         <v>349</v>
       </c>
@@ -4512,7 +4509,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A51" s="176" t="s">
         <v>392</v>
       </c>
@@ -4520,7 +4517,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A52" t="s">
         <v>324</v>
       </c>
@@ -4528,7 +4525,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A53" t="s">
         <v>366</v>
       </c>
@@ -4536,7 +4533,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A54" s="176" t="s">
         <v>387</v>
       </c>
@@ -4544,7 +4541,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A55" s="176" t="s">
         <v>389</v>
       </c>
@@ -4552,7 +4549,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A56" s="176" t="s">
         <v>356</v>
       </c>
@@ -4563,16 +4560,16 @@
         <v>360</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A57" s="176"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A58" s="174" t="s">
         <v>336</v>
       </c>
       <c r="B58" s="175"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A59" t="s">
         <v>349</v>
       </c>
@@ -4580,7 +4577,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A60" s="176" t="s">
         <v>392</v>
       </c>
@@ -4588,7 +4585,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A61" t="s">
         <v>324</v>
       </c>
@@ -4596,7 +4593,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A62" t="s">
         <v>366</v>
       </c>
@@ -4604,7 +4601,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A63" s="176" t="s">
         <v>391</v>
       </c>
@@ -4612,7 +4609,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A64" s="176" t="s">
         <v>388</v>
       </c>
@@ -4620,7 +4617,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A65" s="176" t="s">
         <v>354</v>
       </c>
@@ -4628,33 +4625,33 @@
         <v>355</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A67" s="174" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A68" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A70" s="174" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A71" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A74" s="173" t="s">
         <v>316</v>
       </c>
       <c r="B74" s="177"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A75">
         <v>42</v>
       </c>
@@ -4662,7 +4659,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A76">
         <f>3.41214*10^6</f>
         <v>3412140</v>
@@ -4671,18 +4668,18 @@
         <v>339</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A77">
         <v>61013</v>
       </c>
       <c r="B77" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A79" s="1"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A81" s="182"/>
     </row>
   </sheetData>
@@ -4703,14 +4700,14 @@
       <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.65"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="5" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="20.86328125" style="5" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="45.7265625" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="9.1328125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
       <c r="B1" s="16" t="s">
         <v>386</v>
       </c>
@@ -4817,8 +4814,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.65"/>
+    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C3" s="18" t="s">
         <v>121</v>
       </c>
@@ -4829,7 +4826,7 @@
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
     </row>
-    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C4" s="18" t="s">
         <v>120</v>
       </c>
@@ -4842,7 +4839,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C5" s="18" t="s">
         <v>118</v>
       </c>
@@ -4853,7 +4850,7 @@
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
     </row>
-    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C6" s="18" t="s">
         <v>117</v>
       </c>
@@ -4864,7 +4861,7 @@
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
     </row>
-    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A10" s="7" t="s">
         <v>116</v>
       </c>
@@ -4872,12 +4869,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B11" s="16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B12" s="16" t="s">
         <v>2</v>
       </c>
@@ -4987,7 +4984,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
       <c r="B13" s="14" t="s">
         <v>2</v>
       </c>
@@ -5097,17 +5094,17 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.65">
       <c r="B14" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B15" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A16" s="7" t="s">
         <v>114</v>
       </c>
@@ -5220,7 +5217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A17" s="7" t="s">
         <v>113</v>
       </c>
@@ -5333,7 +5330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A18" s="7" t="s">
         <v>112</v>
       </c>
@@ -5446,7 +5443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A19" s="7" t="s">
         <v>111</v>
       </c>
@@ -5559,7 +5556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A20" s="7" t="s">
         <v>110</v>
       </c>
@@ -5672,7 +5669,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A21" s="7" t="s">
         <v>109</v>
       </c>
@@ -5785,7 +5782,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A22" s="7" t="s">
         <v>108</v>
       </c>
@@ -5898,7 +5895,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A23" s="7" t="s">
         <v>107</v>
       </c>
@@ -6011,7 +6008,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A24" s="7" t="s">
         <v>106</v>
       </c>
@@ -6124,7 +6121,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A25" s="7" t="s">
         <v>105</v>
       </c>
@@ -6237,7 +6234,7 @@
         <v>-1.1E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A26" s="7" t="s">
         <v>104</v>
       </c>
@@ -6350,7 +6347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A27" s="7" t="s">
         <v>103</v>
       </c>
@@ -6463,7 +6460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A28" s="7" t="s">
         <v>102</v>
       </c>
@@ -6576,7 +6573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A29" s="7" t="s">
         <v>100</v>
       </c>
@@ -6689,7 +6686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A30" s="7" t="s">
         <v>99</v>
       </c>
@@ -6802,7 +6799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A31" s="7" t="s">
         <v>98</v>
       </c>
@@ -6915,7 +6912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A32" s="7" t="s">
         <v>97</v>
       </c>
@@ -7028,7 +7025,7 @@
         <v>-2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A33" s="7" t="s">
         <v>96</v>
       </c>
@@ -7141,7 +7138,7 @@
         <v>-2.1599999999999999E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A34" s="7" t="s">
         <v>95</v>
       </c>
@@ -7254,7 +7251,7 @@
         <v>-2.2499999999999999E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A35" s="7" t="s">
         <v>379</v>
       </c>
@@ -7367,7 +7364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A36" s="7" t="s">
         <v>377</v>
       </c>
@@ -7480,7 +7477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A37" s="7" t="s">
         <v>94</v>
       </c>
@@ -7593,7 +7590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A38" s="7" t="s">
         <v>93</v>
       </c>
@@ -7706,7 +7703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A39" s="7" t="s">
         <v>92</v>
       </c>
@@ -7819,7 +7816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A40" s="7" t="s">
         <v>91</v>
       </c>
@@ -7932,7 +7929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A41" s="7" t="s">
         <v>90</v>
       </c>
@@ -8045,7 +8042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A42" s="7" t="s">
         <v>89</v>
       </c>
@@ -8158,7 +8155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A43" s="7" t="s">
         <v>88</v>
       </c>
@@ -8271,7 +8268,7 @@
         <v>1.9699999999999999E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A44" s="7" t="s">
         <v>87</v>
       </c>
@@ -8384,7 +8381,7 @@
         <v>-4.8299999999999998E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A45" s="7" t="s">
         <v>86</v>
       </c>
@@ -8497,7 +8494,7 @@
         <v>-3.1150000000000001E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A46" s="7" t="s">
         <v>85</v>
       </c>
@@ -8610,12 +8607,12 @@
         <v>-1.013E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B47" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A48" s="7" t="s">
         <v>84</v>
       </c>
@@ -8728,7 +8725,7 @@
         <v>-2.4000000000000001E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A49" s="7" t="s">
         <v>83</v>
       </c>
@@ -8841,7 +8838,7 @@
         <v>-3.0000000000000001E-6</v>
       </c>
     </row>
-    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A50" s="7" t="s">
         <v>82</v>
       </c>
@@ -8954,7 +8951,7 @@
         <v>2.3E-5</v>
       </c>
     </row>
-    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A51" s="7" t="s">
         <v>81</v>
       </c>
@@ -9067,12 +9064,12 @@
         <v>-2.7700000000000001E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B53" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A54" s="7" t="s">
         <v>80</v>
       </c>
@@ -9185,7 +9182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A55" s="7" t="s">
         <v>79</v>
       </c>
@@ -9298,7 +9295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A56" s="7" t="s">
         <v>78</v>
       </c>
@@ -9411,7 +9408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A57" s="7" t="s">
         <v>77</v>
       </c>
@@ -9524,7 +9521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A58" s="7" t="s">
         <v>76</v>
       </c>
@@ -9637,7 +9634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A59" s="7" t="s">
         <v>75</v>
       </c>
@@ -9750,7 +9747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A60" s="7" t="s">
         <v>74</v>
       </c>
@@ -9863,12 +9860,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B62" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A63" s="7" t="s">
         <v>73</v>
       </c>
@@ -9981,7 +9978,7 @@
         <v>-1.4100000000000001E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A64" s="7" t="s">
         <v>72</v>
       </c>
@@ -10094,7 +10091,7 @@
         <v>-1.0139999999999999E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A65" s="7" t="s">
         <v>71</v>
       </c>
@@ -10207,7 +10204,7 @@
         <v>-2.1699999999999999E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A66" s="7" t="s">
         <v>70</v>
       </c>
@@ -10320,7 +10317,7 @@
         <v>2.8499999999999999E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A67" s="7" t="s">
         <v>69</v>
       </c>
@@ -10433,7 +10430,7 @@
         <v>2.3E-5</v>
       </c>
     </row>
-    <row r="68" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A68" s="7" t="s">
         <v>68</v>
       </c>
@@ -10546,7 +10543,7 @@
         <v>-5.5000000000000002E-5</v>
       </c>
     </row>
-    <row r="69" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A69" s="7" t="s">
         <v>67</v>
       </c>
@@ -10659,7 +10656,7 @@
         <v>-9.5000000000000005E-5</v>
       </c>
     </row>
-    <row r="70" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A70" s="7" t="s">
         <v>66</v>
       </c>
@@ -10772,7 +10769,7 @@
         <v>2.5799999999999998E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A71" s="7" t="s">
         <v>65</v>
       </c>
@@ -10885,7 +10882,7 @@
         <v>5.7700000000000004E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A72" s="7" t="s">
         <v>64</v>
       </c>
@@ -10998,7 +10995,7 @@
         <v>-1.2830000000000001E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A73" s="7" t="s">
         <v>63</v>
       </c>
@@ -11111,7 +11108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A74" s="7" t="s">
         <v>62</v>
       </c>
@@ -11224,7 +11221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A76" s="7" t="s">
         <v>61</v>
       </c>
@@ -11337,8 +11334,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.8"/>
+    <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B78" s="183" t="s">
         <v>57</v>
       </c>
@@ -11378,37 +11375,37 @@
       <c r="AJ78" s="183"/>
       <c r="AK78" s="183"/>
     </row>
-    <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B79" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="80" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B80" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B81" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B82" s="6" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="83" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B83" s="6" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="84" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B84" s="6" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="85" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B85" s="6" t="s">
         <v>372</v>
       </c>
@@ -11428,35 +11425,35 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.1328125" customWidth="1"/>
+    <col min="2" max="2" width="13.40625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.40625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" customWidth="1"/>
+    <col min="7" max="7" width="13.40625" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.40625" customWidth="1"/>
+    <col min="12" max="12" width="12.40625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.40625" customWidth="1"/>
+    <col min="23" max="23" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="15.75" x14ac:dyDescent="0.75">
       <c r="A1" s="19" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A2" s="20" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A3" s="21" t="s">
         <v>126</v>
       </c>
@@ -11479,7 +11476,7 @@
       </c>
       <c r="I3" s="25"/>
     </row>
-    <row r="4" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="26.75" x14ac:dyDescent="0.75">
       <c r="A4" s="26"/>
       <c r="B4" s="27" t="s">
         <v>302</v>
@@ -11504,7 +11501,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A5" s="31" t="s">
         <v>137</v>
       </c>
@@ -11521,7 +11518,7 @@
       <c r="H5" s="34"/>
       <c r="I5" s="35"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A6" s="36" t="s">
         <v>139</v>
       </c>
@@ -11542,7 +11539,7 @@
       <c r="H6" s="39"/>
       <c r="I6" s="40"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A7" s="41" t="s">
         <v>142</v>
       </c>
@@ -11571,7 +11568,7 @@
         <v>0.93726057101554028</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A8" s="41" t="s">
         <v>143</v>
       </c>
@@ -11600,7 +11597,7 @@
         <v>0.93500000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A9" s="41" t="s">
         <v>144</v>
       </c>
@@ -11629,7 +11626,7 @@
         <v>0.93500000000000016</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A10" s="41" t="s">
         <v>145</v>
       </c>
@@ -11658,7 +11655,7 @@
         <v>0.93500000000000016</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A11" s="41" t="s">
         <v>146</v>
       </c>
@@ -11695,7 +11692,7 @@
       <c r="R11" s="46"/>
       <c r="S11" s="52"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A12" s="41" t="s">
         <v>147</v>
       </c>
@@ -11724,7 +11721,7 @@
         <v>0.93500000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>148</v>
       </c>
@@ -11753,7 +11750,7 @@
         <v>0.93726057101554028</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>149</v>
       </c>
@@ -11782,7 +11779,7 @@
         <v>0.93726057101554017</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A15" s="41" t="s">
         <v>150</v>
       </c>
@@ -11819,7 +11816,7 @@
       <c r="V15" s="57"/>
       <c r="W15" s="53"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A16" s="41" t="s">
         <v>151</v>
       </c>
@@ -11853,7 +11850,7 @@
       <c r="V16" s="57"/>
       <c r="W16" s="53"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A17" s="41" t="s">
         <v>152</v>
       </c>
@@ -11890,7 +11887,7 @@
       <c r="V17" s="57"/>
       <c r="W17" s="53"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A18" s="41" t="s">
         <v>153</v>
       </c>
@@ -11924,7 +11921,7 @@
       <c r="V18" s="57"/>
       <c r="W18" s="53"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A19" s="41" t="s">
         <v>154</v>
       </c>
@@ -11958,7 +11955,7 @@
       <c r="M19" s="57"/>
       <c r="N19" s="53"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A20" s="41" t="s">
         <v>303</v>
       </c>
@@ -11988,7 +11985,7 @@
       </c>
       <c r="W20" s="53"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A21" s="59" t="s">
         <v>406</v>
       </c>
@@ -12015,7 +12012,7 @@
       </c>
       <c r="I21" s="47"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A22" s="41" t="s">
         <v>155</v>
       </c>
@@ -12044,7 +12041,7 @@
         <v>0.93499781627602274</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A23" s="41" t="s">
         <v>156</v>
       </c>
@@ -12073,7 +12070,7 @@
         <v>0.93499781627602274</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A24" s="41" t="s">
         <v>157</v>
       </c>
@@ -12102,7 +12099,7 @@
         <v>0.93476175247841387</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A25" s="41" t="s">
         <v>407</v>
       </c>
@@ -12131,7 +12128,7 @@
         <v>0.93404711473172097</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A26" s="41" t="s">
         <v>158</v>
       </c>
@@ -12160,7 +12157,7 @@
         <v>0.93500003751584637</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A27" s="41" t="s">
         <v>159</v>
       </c>
@@ -12189,7 +12186,7 @@
         <v>0.93500003751584626</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A28" s="41" t="s">
         <v>160</v>
       </c>
@@ -12218,7 +12215,7 @@
         <v>0.93135126106564226</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A29" s="41" t="s">
         <v>161</v>
       </c>
@@ -12247,7 +12244,7 @@
         <v>0.93499781627602263</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A30" s="41" t="s">
         <v>162</v>
       </c>
@@ -12276,7 +12273,7 @@
         <v>0.93499781627602263</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A31" s="41" t="s">
         <v>163</v>
       </c>
@@ -12305,7 +12302,7 @@
         <v>0.87806748466257667</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.75">
       <c r="A32" s="41" t="s">
         <v>164</v>
       </c>
@@ -12334,7 +12331,7 @@
         <v>0.90299302022950434</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A33" s="41" t="s">
         <v>165</v>
       </c>
@@ -12363,7 +12360,7 @@
         <v>0.92051300964428628</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A34" s="41" t="s">
         <v>166</v>
       </c>
@@ -12392,7 +12389,7 @@
         <v>0.92867915675168411</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A35" s="41" t="s">
         <v>167</v>
       </c>
@@ -12421,7 +12418,7 @@
         <v>0.93364967025896739</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A36" s="41" t="s">
         <v>168</v>
       </c>
@@ -12450,7 +12447,7 @@
         <v>0.9293293950333662</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A37" s="41" t="s">
         <v>169</v>
       </c>
@@ -12479,7 +12476,7 @@
         <v>0.88092431030417351</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A38" s="41" t="s">
         <v>170</v>
       </c>
@@ -12508,7 +12505,7 @@
         <v>0.91165189789710355</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A39" s="41" t="s">
         <v>171</v>
       </c>
@@ -12537,7 +12534,7 @@
         <v>0.91165189789710355</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A40" s="41" t="s">
         <v>172</v>
       </c>
@@ -12566,7 +12563,7 @@
         <v>0.93427633635511098</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A41" s="41" t="s">
         <v>173</v>
       </c>
@@ -12595,7 +12592,7 @@
         <v>0.95108821041298164</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A42" s="41" t="s">
         <v>174</v>
       </c>
@@ -12624,7 +12621,7 @@
         <v>0.93427633635511098</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A43" s="41" t="s">
         <v>175</v>
       </c>
@@ -12653,7 +12650,7 @@
         <v>0.93938096730547249</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A44" s="41" t="s">
         <v>176</v>
       </c>
@@ -12682,7 +12679,7 @@
         <v>0.92840083590406852</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A45" t="s">
         <v>177</v>
       </c>
@@ -12711,7 +12708,7 @@
         <v>0.93361506882395562</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A46" s="41" t="s">
         <v>178</v>
       </c>
@@ -12740,7 +12737,7 @@
         <v>0.93361506882395551</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A47" s="41" t="s">
         <v>408</v>
       </c>
@@ -12769,7 +12766,7 @@
         <v>0.93361506882395551</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A48" s="41" t="s">
         <v>179</v>
       </c>
@@ -12798,7 +12795,7 @@
         <v>0.93500003751584626</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A49" s="41" t="s">
         <v>180</v>
       </c>
@@ -12827,7 +12824,7 @@
         <v>0.84675180455302612</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A50" s="41" t="s">
         <v>181</v>
       </c>
@@ -12856,7 +12853,7 @@
         <v>0.92494808662118067</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A51" s="41" t="s">
         <v>182</v>
       </c>
@@ -12885,7 +12882,7 @@
         <v>0.92528460728977324</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A52" s="41" t="s">
         <v>183</v>
       </c>
@@ -12914,7 +12911,7 @@
         <v>0.92548586165607438</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A53" s="41" t="s">
         <v>184</v>
       </c>
@@ -12943,7 +12940,7 @@
         <v>0.92007362914163926</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A54" s="41" t="s">
         <v>185</v>
       </c>
@@ -12972,7 +12969,7 @@
         <v>0.91375811688311692</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A55" s="41" t="s">
         <v>186</v>
       </c>
@@ -13001,7 +12998,7 @@
         <v>0.92923017182797785</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A56" s="41" t="s">
         <v>187</v>
       </c>
@@ -13030,7 +13027,7 @@
         <v>0.92157077225989936</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A57" s="41" t="s">
         <v>188</v>
       </c>
@@ -13057,7 +13054,7 @@
         <v>0.92932939503336609</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A58" s="36" t="s">
         <v>189</v>
       </c>
@@ -13086,7 +13083,7 @@
         <v>0.93722267739953979</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A59" s="41" t="s">
         <v>191</v>
       </c>
@@ -13109,7 +13106,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A60" s="41" t="s">
         <v>194</v>
       </c>
@@ -13138,7 +13135,7 @@
         <v>0.90266299357208446</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A61" s="41" t="s">
         <v>195</v>
       </c>
@@ -13167,7 +13164,7 @@
         <v>0.9009009009009008</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A62" s="41" t="s">
         <v>196</v>
       </c>
@@ -13196,7 +13193,7 @@
         <v>0.84548104956268222</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A63" s="41" t="s">
         <v>197</v>
       </c>
@@ -13217,7 +13214,7 @@
       </c>
       <c r="I63" s="47"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A64" s="36" t="s">
         <v>190</v>
       </c>
@@ -13246,7 +13243,7 @@
         <v>0.90586790472651468</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A65" s="41" t="s">
         <v>198</v>
       </c>
@@ -13267,7 +13264,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A66" s="59" t="s">
         <v>200</v>
       </c>
@@ -13293,7 +13290,7 @@
       <c r="I66" s="81"/>
       <c r="K66" s="82"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A67" s="59" t="s">
         <v>201</v>
       </c>
@@ -13321,7 +13318,7 @@
       </c>
       <c r="K67" s="82"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A68" s="59" t="s">
         <v>202</v>
       </c>
@@ -13349,7 +13346,7 @@
       </c>
       <c r="K68" s="82"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A69" s="59" t="s">
         <v>203</v>
       </c>
@@ -13377,7 +13374,7 @@
       </c>
       <c r="K69" s="82"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A70" s="59" t="s">
         <v>204</v>
       </c>
@@ -13405,7 +13402,7 @@
       </c>
       <c r="K70" s="82"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A71" s="41" t="s">
         <v>205</v>
       </c>
@@ -13434,7 +13431,7 @@
       <c r="K71" s="82"/>
       <c r="L71" s="82"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A72" s="41" t="s">
         <v>206</v>
       </c>
@@ -13462,7 +13459,7 @@
       </c>
       <c r="K72" s="82"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A73" s="41" t="s">
         <v>207</v>
       </c>
@@ -13489,7 +13486,7 @@
         <v>0.94242199100000001</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="12.65" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A74" s="41" t="s">
         <v>208</v>
       </c>
@@ -13517,7 +13514,7 @@
       </c>
       <c r="K74" s="84"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A75" s="41" t="s">
         <v>409</v>
       </c>
@@ -13545,7 +13542,7 @@
       </c>
       <c r="K75" s="84"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A76" s="41" t="s">
         <v>209</v>
       </c>
@@ -13572,7 +13569,7 @@
         <v>0.93173565722585328</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A77" s="41" t="s">
         <v>210</v>
       </c>
@@ -13600,7 +13597,7 @@
       </c>
       <c r="K77" s="85"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A78" s="41" t="s">
         <v>211</v>
       </c>
@@ -13628,7 +13625,7 @@
       </c>
       <c r="K78" s="84"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A79" s="41" t="s">
         <v>212</v>
       </c>
@@ -13655,7 +13652,7 @@
         <v>0.93680161201685286</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A80" s="41" t="s">
         <v>213</v>
       </c>
@@ -13682,7 +13679,7 @@
         <v>0.93292760238366934</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A81" s="41" t="s">
         <v>214</v>
       </c>
@@ -13709,7 +13706,7 @@
         <v>0.96554227633195577</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A82" s="41" t="s">
         <v>410</v>
       </c>
@@ -13736,7 +13733,7 @@
         <v>0.93359512366662756</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A83" s="59" t="s">
         <v>215</v>
       </c>
@@ -13759,7 +13756,7 @@
       </c>
       <c r="I83" s="88"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A84" s="89" t="s">
         <v>216</v>
       </c>
@@ -13782,7 +13779,7 @@
         <v>0.85292563033160751</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A85" s="89" t="s">
         <v>217</v>
       </c>
@@ -13805,7 +13802,7 @@
         <v>0.88047037071579148</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A86" s="89" t="s">
         <v>218</v>
       </c>
@@ -13832,7 +13829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A87" s="92" t="s">
         <v>219</v>
       </c>
@@ -13859,7 +13856,7 @@
         <v>0.90447216306662592</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A88" s="93" t="s">
         <v>220</v>
       </c>
@@ -13886,7 +13883,7 @@
         <v>0.94150280898876404</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A89" t="s">
         <v>221</v>
       </c>
@@ -13913,7 +13910,7 @@
         <v>0.94150280898876404</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A90" s="20" t="s">
         <v>222</v>
       </c>
@@ -13940,7 +13937,7 @@
         <v>0.8252427184466018</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A91" t="s">
         <v>223</v>
       </c>
@@ -13967,7 +13964,7 @@
         <v>0.87681159420289856</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A92" s="104" t="s">
         <v>411</v>
       </c>
@@ -14001,7 +13998,7 @@
       <c r="M92" s="107"/>
       <c r="N92" s="108"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A93" s="109" t="s">
         <v>412</v>
       </c>
@@ -14027,19 +14024,19 @@
       <c r="M93" s="111"/>
       <c r="N93" s="112"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A94" s="113"/>
       <c r="B94" s="114"/>
       <c r="N94" s="115"/>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A95" s="113" t="s">
         <v>224</v>
       </c>
       <c r="B95" s="114"/>
       <c r="N95" s="115"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A96" s="109" t="s">
         <v>225</v>
       </c>
@@ -14057,7 +14054,7 @@
       <c r="M96" s="117"/>
       <c r="N96" s="118"/>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A97" s="119" t="s">
         <v>226</v>
       </c>
@@ -14101,7 +14098,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A98" s="2" t="s">
         <v>233</v>
       </c>
@@ -14145,7 +14142,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A99" s="120" t="s">
         <v>234</v>
       </c>
@@ -14189,7 +14186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A100" s="109" t="s">
         <v>235</v>
       </c>
@@ -14233,7 +14230,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A101" s="113" t="s">
         <v>236</v>
       </c>
@@ -14277,19 +14274,19 @@
         <v>270</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A102" s="113"/>
       <c r="B102" s="114"/>
       <c r="G102" s="115"/>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A103" s="113" t="s">
         <v>237</v>
       </c>
       <c r="B103" s="114"/>
       <c r="G103" s="115"/>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A104" s="113" t="s">
         <v>238</v>
       </c>
@@ -14312,7 +14309,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A105" s="109" t="s">
         <v>233</v>
       </c>
@@ -14333,7 +14330,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A106" t="s">
         <v>242</v>
       </c>
@@ -14356,7 +14353,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A107" s="20" t="s">
         <v>243</v>
       </c>
@@ -14379,7 +14376,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A108" s="104" t="s">
         <v>244</v>
       </c>
@@ -14402,7 +14399,7 @@
         <v>-87</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A109" s="113" t="s">
         <v>245</v>
       </c>
@@ -14425,7 +14422,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A110" s="113" t="s">
         <v>246</v>
       </c>
@@ -14448,17 +14445,17 @@
         <v>-71</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A111" s="113"/>
       <c r="B111" s="129"/>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A112" s="109" t="s">
         <v>247</v>
       </c>
       <c r="B112" s="130"/>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A113" t="s">
         <v>248</v>
       </c>
@@ -14466,7 +14463,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A114" s="20" t="s">
         <v>249</v>
       </c>
@@ -14474,7 +14471,7 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A115" t="s">
         <v>250</v>
       </c>
@@ -14482,7 +14479,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A116" t="s">
         <v>251</v>
       </c>
@@ -14495,7 +14492,7 @@
       <c r="R116" s="133"/>
       <c r="V116" s="133"/>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A117" t="s">
         <v>252</v>
       </c>
@@ -14508,7 +14505,7 @@
       <c r="R117" s="136"/>
       <c r="V117" s="136"/>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.75">
       <c r="B118" s="137"/>
       <c r="C118" s="138"/>
       <c r="D118" s="139"/>
@@ -14528,7 +14525,7 @@
       <c r="W118" s="140"/>
       <c r="X118" s="139"/>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A119" t="s">
         <v>253</v>
       </c>
@@ -14551,7 +14548,7 @@
       <c r="W119" s="142"/>
       <c r="X119" s="143"/>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:24" x14ac:dyDescent="0.75">
       <c r="B120" s="144"/>
       <c r="C120" s="136"/>
       <c r="D120" s="145"/>
@@ -14571,7 +14568,7 @@
       <c r="W120" s="136"/>
       <c r="X120" s="145"/>
     </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:24" x14ac:dyDescent="0.75">
       <c r="B121" s="144">
         <v>10</v>
       </c>
@@ -14603,7 +14600,7 @@
       <c r="W121" s="136"/>
       <c r="X121" s="145"/>
     </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:24" x14ac:dyDescent="0.75">
       <c r="B122" s="144">
         <v>10</v>
       </c>
@@ -14635,7 +14632,7 @@
       <c r="W122" s="136"/>
       <c r="X122" s="145"/>
     </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:24" x14ac:dyDescent="0.75">
       <c r="B123" s="144" t="s">
         <v>254</v>
       </c>
@@ -14691,7 +14688,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:24" x14ac:dyDescent="0.75">
       <c r="B124" s="144">
         <v>1990</v>
       </c>
@@ -14747,7 +14744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:24" x14ac:dyDescent="0.75">
       <c r="B125" s="144">
         <v>1995</v>
       </c>
@@ -14803,7 +14800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:24" x14ac:dyDescent="0.75">
       <c r="B126" s="149">
         <v>2000</v>
       </c>
@@ -14859,7 +14856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:24" x14ac:dyDescent="0.75">
       <c r="B127">
         <v>2005</v>
       </c>
@@ -14915,7 +14912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A128" s="20"/>
       <c r="B128">
         <v>2010</v>
@@ -14972,7 +14969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A129" s="152"/>
       <c r="B129" s="153">
         <v>2015</v>
@@ -15030,7 +15027,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A130" s="155"/>
       <c r="B130" s="156">
         <v>2017</v>
@@ -15088,7 +15085,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="131" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A131" s="155"/>
       <c r="B131" s="159">
         <v>2020</v>
@@ -15102,7 +15099,7 @@
       <c r="E131" s="157"/>
       <c r="F131" s="160"/>
     </row>
-    <row r="132" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A132" s="155"/>
       <c r="B132" s="159"/>
       <c r="C132" s="159"/>
@@ -15110,7 +15107,7 @@
       <c r="E132" s="159"/>
       <c r="F132" s="160"/>
     </row>
-    <row r="133" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A133" s="155" t="s">
         <v>262</v>
       </c>
@@ -15120,7 +15117,7 @@
       <c r="E133" s="156"/>
       <c r="F133" s="158"/>
     </row>
-    <row r="134" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A134" s="161" t="s">
         <v>263</v>
       </c>
@@ -15140,7 +15137,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="135" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A135" t="s">
         <v>269</v>
       </c>
@@ -15160,7 +15157,7 @@
         <v>907184.74</v>
       </c>
     </row>
-    <row r="136" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A136" s="152" t="s">
         <v>270</v>
       </c>
@@ -15180,7 +15177,7 @@
         <v>907.18474000000003</v>
       </c>
     </row>
-    <row r="137" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A137" s="155" t="s">
         <v>271</v>
       </c>
@@ -15200,7 +15197,7 @@
         <v>0.90718474000000004</v>
       </c>
     </row>
-    <row r="138" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A138" s="155" t="s">
         <v>272</v>
       </c>
@@ -15220,7 +15217,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="139" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A139" s="155" t="s">
         <v>273</v>
       </c>
@@ -15240,7 +15237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A140" s="155"/>
       <c r="B140" s="136"/>
       <c r="C140" s="159"/>
@@ -15248,7 +15245,7 @@
       <c r="E140" s="156"/>
       <c r="F140" s="160"/>
     </row>
-    <row r="141" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A141" s="161" t="s">
         <v>274</v>
       </c>
@@ -15268,7 +15265,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A142" t="s">
         <v>280</v>
       </c>
@@ -15288,7 +15285,7 @@
         <v>2.8316846999999999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A143" s="152" t="s">
         <v>281</v>
       </c>
@@ -15311,7 +15308,7 @@
       <c r="H143" s="153"/>
       <c r="I143" s="154"/>
     </row>
-    <row r="144" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A144" s="155" t="s">
         <v>282</v>
       </c>
@@ -15334,7 +15331,7 @@
       <c r="H144" s="156"/>
       <c r="I144" s="115"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A145" s="155" t="s">
         <v>283</v>
       </c>
@@ -15357,7 +15354,7 @@
       <c r="H145" s="156"/>
       <c r="I145" s="115"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A146" s="155" t="s">
         <v>284</v>
       </c>
@@ -15380,7 +15377,7 @@
       <c r="H146" s="156"/>
       <c r="I146" s="115"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A147" s="155"/>
       <c r="B147" s="159"/>
       <c r="C147" s="157"/>
@@ -15391,7 +15388,7 @@
       <c r="H147" s="156"/>
       <c r="I147" s="115"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A148" s="155" t="s">
         <v>285</v>
       </c>
@@ -15420,7 +15417,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A149" s="155" t="s">
         <v>294</v>
       </c>
@@ -15449,7 +15446,7 @@
         <v>2684519.5376862194</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A150" s="155" t="s">
         <v>295</v>
       </c>
@@ -15478,7 +15475,7 @@
         <v>2684.5195376862198</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A151" s="161" t="s">
         <v>296</v>
       </c>
@@ -15507,7 +15504,7 @@
         <v>2.6845195376862194</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A152" t="s">
         <v>297</v>
       </c>
@@ -15536,7 +15533,7 @@
         <v>745.69987157950538</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A153" t="s">
         <v>298</v>
       </c>
@@ -15565,7 +15562,7 @@
         <v>0.74569987157950535</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A154" t="s">
         <v>299</v>
       </c>
@@ -15594,7 +15591,7 @@
         <v>2544.4335839531336</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A155" t="s">
         <v>300</v>
       </c>
@@ -15623,7 +15620,7 @@
         <v>2.5444335839531337E-3</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A156" t="s">
         <v>301</v>
       </c>
@@ -15652,7 +15649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A158" t="s">
         <v>413</v>
       </c>
@@ -15672,7 +15669,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A159" t="s">
         <v>414</v>
       </c>
@@ -15692,7 +15689,7 @@
         <v>1609340</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A160" t="s">
         <v>415</v>
       </c>
@@ -15712,7 +15709,7 @@
         <v>1609.34</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A161" t="s">
         <v>416</v>
       </c>
@@ -15732,7 +15729,7 @@
         <v>1.60934</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A162" t="s">
         <v>417</v>
       </c>
@@ -15752,7 +15749,7 @@
         <v>5280</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A163" t="s">
         <v>418</v>
       </c>
@@ -15800,127 +15797,117 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AI22"/>
+  <dimension ref="A1:AF22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="35" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.86328125" customWidth="1"/>
+    <col min="2" max="32" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>404</v>
       </c>
       <c r="B1">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="C1">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="D1">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="E1">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="F1">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="G1">
-        <v>2022</v>
+        <v>2025</v>
       </c>
       <c r="H1">
-        <v>2023</v>
+        <v>2026</v>
       </c>
       <c r="I1">
-        <v>2024</v>
+        <v>2027</v>
       </c>
       <c r="J1">
-        <v>2025</v>
+        <v>2028</v>
       </c>
       <c r="K1">
-        <v>2026</v>
+        <v>2029</v>
       </c>
       <c r="L1">
-        <v>2027</v>
+        <v>2030</v>
       </c>
       <c r="M1">
-        <v>2028</v>
+        <v>2031</v>
       </c>
       <c r="N1">
-        <v>2029</v>
+        <v>2032</v>
       </c>
       <c r="O1">
-        <v>2030</v>
+        <v>2033</v>
       </c>
       <c r="P1">
-        <v>2031</v>
+        <v>2034</v>
       </c>
       <c r="Q1">
-        <v>2032</v>
+        <v>2035</v>
       </c>
       <c r="R1">
-        <v>2033</v>
+        <v>2036</v>
       </c>
       <c r="S1">
-        <v>2034</v>
+        <v>2037</v>
       </c>
       <c r="T1">
-        <v>2035</v>
+        <v>2038</v>
       </c>
       <c r="U1">
-        <v>2036</v>
+        <v>2039</v>
       </c>
       <c r="V1">
-        <v>2037</v>
+        <v>2040</v>
       </c>
       <c r="W1">
-        <v>2038</v>
+        <v>2041</v>
       </c>
       <c r="X1">
-        <v>2039</v>
+        <v>2042</v>
       </c>
       <c r="Y1">
-        <v>2040</v>
+        <v>2043</v>
       </c>
       <c r="Z1">
-        <v>2041</v>
+        <v>2044</v>
       </c>
       <c r="AA1">
-        <v>2042</v>
+        <v>2045</v>
       </c>
       <c r="AB1">
-        <v>2043</v>
+        <v>2046</v>
       </c>
       <c r="AC1">
-        <v>2044</v>
+        <v>2047</v>
       </c>
       <c r="AD1">
-        <v>2045</v>
+        <v>2048</v>
       </c>
       <c r="AE1">
-        <v>2046</v>
+        <v>2049</v>
       </c>
       <c r="AF1">
-        <v>2047</v>
-      </c>
-      <c r="AG1">
-        <v>2048</v>
-      </c>
-      <c r="AH1">
-        <v>2049</v>
-      </c>
-      <c r="AI1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>346</v>
       </c>
@@ -16048,307 +16035,271 @@
         <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
-      <c r="AG2">
-        <f>About!$A$76*10^6</f>
-        <v>3412140000000</v>
-      </c>
-      <c r="AH2">
-        <f>About!$A$76*10^6</f>
-        <v>3412140000000</v>
-      </c>
-      <c r="AI2">
-        <f>About!$A$76*10^6</f>
-        <v>3412140000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>323</v>
       </c>
       <c r="B3">
-        <f>'AEO Table 73'!C66*10^12</f>
-        <v>19437477000000</v>
-      </c>
-      <c r="C3">
-        <f>'AEO Table 73'!D66*10^12</f>
-        <v>19706896000000</v>
-      </c>
-      <c r="D3">
-        <f>'AEO Table 73'!E66*10^12</f>
-        <v>19588093000000</v>
-      </c>
-      <c r="E3">
         <f>'AEO Table 73'!F66*10^12</f>
         <v>19676338000000</v>
       </c>
-      <c r="F3">
+      <c r="C3">
         <f>'AEO Table 73'!G66*10^12</f>
         <v>19593861000000</v>
       </c>
-      <c r="G3">
+      <c r="D3">
         <f>'AEO Table 73'!H66*10^12</f>
         <v>19763271000000</v>
       </c>
-      <c r="H3">
+      <c r="E3">
         <f>'AEO Table 73'!I66*10^12</f>
         <v>19874037000000</v>
       </c>
-      <c r="I3">
+      <c r="F3">
         <f>'AEO Table 73'!J66*10^12</f>
         <v>19832983000000</v>
       </c>
-      <c r="J3">
+      <c r="G3">
         <f>'AEO Table 73'!K66*10^12</f>
         <v>19854052000000</v>
       </c>
-      <c r="K3">
+      <c r="H3">
         <f>'AEO Table 73'!L66*10^12</f>
         <v>19849159000000</v>
       </c>
-      <c r="L3">
+      <c r="I3">
         <f>'AEO Table 73'!M66*10^12</f>
         <v>19841606000000</v>
       </c>
-      <c r="M3">
+      <c r="J3">
         <f>'AEO Table 73'!N66*10^12</f>
         <v>19838451000000</v>
       </c>
-      <c r="N3">
+      <c r="K3">
         <f>'AEO Table 73'!O66*10^12</f>
         <v>19782232000000</v>
       </c>
-      <c r="O3">
+      <c r="L3">
         <f>'AEO Table 73'!P66*10^12</f>
         <v>19750866000000</v>
       </c>
-      <c r="P3">
+      <c r="M3">
         <f>'AEO Table 73'!Q66*10^12</f>
         <v>19757530000000</v>
       </c>
-      <c r="Q3">
+      <c r="N3">
         <f>'AEO Table 73'!R66*10^12</f>
         <v>19792145000000</v>
       </c>
-      <c r="R3">
+      <c r="O3">
         <f>'AEO Table 73'!S66*10^12</f>
         <v>19787580000000</v>
       </c>
-      <c r="S3">
+      <c r="P3">
         <f>'AEO Table 73'!T66*10^12</f>
         <v>19792101000000</v>
       </c>
-      <c r="T3">
+      <c r="Q3">
         <f>'AEO Table 73'!U66*10^12</f>
         <v>19801369000000</v>
       </c>
-      <c r="U3">
+      <c r="R3">
         <f>'AEO Table 73'!V66*10^12</f>
         <v>19790552000000</v>
       </c>
-      <c r="V3">
+      <c r="S3">
         <f>'AEO Table 73'!W66*10^12</f>
         <v>19813770000000</v>
       </c>
-      <c r="W3">
+      <c r="T3">
         <f>'AEO Table 73'!X66*10^12</f>
         <v>19823812000000</v>
       </c>
-      <c r="X3">
+      <c r="U3">
         <f>'AEO Table 73'!Y66*10^12</f>
         <v>19819962000000</v>
       </c>
-      <c r="Y3">
+      <c r="V3">
         <f>'AEO Table 73'!Z66*10^12</f>
         <v>19817593000000</v>
       </c>
-      <c r="Z3">
+      <c r="W3">
         <f>'AEO Table 73'!AA66*10^12</f>
         <v>19814734000000</v>
       </c>
-      <c r="AA3">
+      <c r="X3">
         <f>'AEO Table 73'!AB66*10^12</f>
         <v>19808729000000</v>
       </c>
-      <c r="AB3">
+      <c r="Y3">
         <f>'AEO Table 73'!AC66*10^12</f>
         <v>19816940000000</v>
       </c>
-      <c r="AC3">
+      <c r="Z3">
         <f>'AEO Table 73'!AD66*10^12</f>
         <v>19822159000000</v>
       </c>
-      <c r="AD3">
+      <c r="AA3">
         <f>'AEO Table 73'!AE66*10^12</f>
         <v>19832388000000</v>
       </c>
-      <c r="AE3">
+      <c r="AB3">
         <f>'AEO Table 73'!AF66*10^12</f>
         <v>19856539000000</v>
       </c>
-      <c r="AF3">
+      <c r="AC3">
         <f>'AEO Table 73'!AG66*10^12</f>
         <v>19880623000000</v>
       </c>
-      <c r="AG3">
+      <c r="AD3">
         <f>'AEO Table 73'!AH66*10^12</f>
         <v>19899242000000</v>
       </c>
-      <c r="AH3">
+      <c r="AE3">
         <f>'AEO Table 73'!AI66*10^12</f>
         <v>19884989000000</v>
       </c>
-      <c r="AI3">
+      <c r="AF3">
         <f>'AEO Table 73'!AJ66*10^12</f>
         <v>19887484000000</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>324</v>
       </c>
       <c r="B4">
-        <f>'AEO Table 73'!C54*10^15</f>
-        <v>1036999999999999.9</v>
-      </c>
-      <c r="C4">
-        <f>'AEO Table 73'!D54*10^15</f>
-        <v>1036999999999999.9</v>
-      </c>
-      <c r="D4">
-        <f>'AEO Table 73'!E54*10^15</f>
-        <v>1036999999999999.9</v>
-      </c>
-      <c r="E4">
         <f>'AEO Table 73'!F54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="F4">
+      <c r="C4">
         <f>'AEO Table 73'!G54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="G4">
+      <c r="D4">
         <f>'AEO Table 73'!H54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="H4">
+      <c r="E4">
         <f>'AEO Table 73'!I54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="I4">
+      <c r="F4">
         <f>'AEO Table 73'!J54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="J4">
+      <c r="G4">
         <f>'AEO Table 73'!K54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="K4">
+      <c r="H4">
         <f>'AEO Table 73'!L54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="L4">
+      <c r="I4">
         <f>'AEO Table 73'!M54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="M4">
+      <c r="J4">
         <f>'AEO Table 73'!N54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="N4">
+      <c r="K4">
         <f>'AEO Table 73'!O54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="O4">
+      <c r="L4">
         <f>'AEO Table 73'!P54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="P4">
+      <c r="M4">
         <f>'AEO Table 73'!Q54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="Q4">
+      <c r="N4">
         <f>'AEO Table 73'!R54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="R4">
+      <c r="O4">
         <f>'AEO Table 73'!S54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="S4">
+      <c r="P4">
         <f>'AEO Table 73'!T54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="T4">
+      <c r="Q4">
         <f>'AEO Table 73'!U54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="U4">
+      <c r="R4">
         <f>'AEO Table 73'!V54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="V4">
+      <c r="S4">
         <f>'AEO Table 73'!W54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="W4">
+      <c r="T4">
         <f>'AEO Table 73'!X54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="X4">
+      <c r="U4">
         <f>'AEO Table 73'!Y54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="Y4">
+      <c r="V4">
         <f>'AEO Table 73'!Z54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="Z4">
+      <c r="W4">
         <f>'AEO Table 73'!AA54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="AA4">
+      <c r="X4">
         <f>'AEO Table 73'!AB54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="AB4">
+      <c r="Y4">
         <f>'AEO Table 73'!AC54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="AC4">
+      <c r="Z4">
         <f>'AEO Table 73'!AD54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="AD4">
+      <c r="AA4">
         <f>'AEO Table 73'!AE54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="AE4">
+      <c r="AB4">
         <f>'AEO Table 73'!AF54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="AF4">
+      <c r="AC4">
         <f>'AEO Table 73'!AG54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="AG4">
+      <c r="AD4">
         <f>'AEO Table 73'!AH54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="AH4">
+      <c r="AE4">
         <f>'AEO Table 73'!AI54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
-      <c r="AI4">
+      <c r="AF4">
         <f>'AEO Table 73'!AJ54*10^15</f>
         <v>1036999999999999.9</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>340</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:AI5" si="0">10^12</f>
+        <f t="shared" ref="B5:AF5" si="0">10^12</f>
         <v>1000000000000</v>
       </c>
       <c r="C5">
@@ -16471,20 +16422,8 @@
         <f t="shared" si="0"/>
         <v>1000000000000</v>
       </c>
-      <c r="AG5">
-        <f t="shared" si="0"/>
-        <v>1000000000000</v>
-      </c>
-      <c r="AH5">
-        <f t="shared" si="0"/>
-        <v>1000000000000</v>
-      </c>
-      <c r="AI5">
-        <f t="shared" si="0"/>
-        <v>1000000000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>341</v>
       </c>
@@ -16581,17 +16520,8 @@
       <c r="AF6">
         <v>0</v>
       </c>
-      <c r="AG6">
-        <v>0</v>
-      </c>
-      <c r="AH6">
-        <v>0</v>
-      </c>
-      <c r="AI6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>342</v>
       </c>
@@ -16688,17 +16618,8 @@
       <c r="AF7">
         <v>0</v>
       </c>
-      <c r="AG7">
-        <v>0</v>
-      </c>
-      <c r="AH7">
-        <v>0</v>
-      </c>
-      <c r="AI7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>343</v>
       </c>
@@ -16795,17 +16716,8 @@
       <c r="AF8">
         <v>0</v>
       </c>
-      <c r="AG8">
-        <v>0</v>
-      </c>
-      <c r="AH8">
-        <v>0</v>
-      </c>
-      <c r="AI8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>325</v>
       </c>
@@ -16933,20 +16845,8 @@
         <f>'GREET1 Fuel_Specs'!$D$81*10^6</f>
         <v>17906000000000</v>
       </c>
-      <c r="AG9">
-        <f>'GREET1 Fuel_Specs'!$D$81*10^6</f>
-        <v>17906000000000</v>
-      </c>
-      <c r="AH9">
-        <f>'GREET1 Fuel_Specs'!$D$81*10^6</f>
-        <v>17906000000000</v>
-      </c>
-      <c r="AI9">
-        <f>'GREET1 Fuel_Specs'!$D$81*10^6</f>
-        <v>17906000000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>326</v>
       </c>
@@ -17074,20 +16974,8 @@
         <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
         <v>5810700000000</v>
       </c>
-      <c r="AG10">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-      <c r="AH10">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-      <c r="AI10">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>327</v>
       </c>
@@ -17215,25 +17103,14 @@
         <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
         <v>5810700000000</v>
       </c>
-      <c r="AG11">
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.75">
+      <c r="A12" t="s">
+        <v>328</v>
+      </c>
+      <c r="B12">
         <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
         <v>5810700000000</v>
-      </c>
-      <c r="AH11">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-      <c r="AI11">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>328</v>
-      </c>
-      <c r="B12" t="s">
-        <v>424</v>
       </c>
       <c r="C12">
         <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
@@ -17355,20 +17232,8 @@
         <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
         <v>5810700000000</v>
       </c>
-      <c r="AG12">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-      <c r="AH12">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-      <c r="AI12">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>329</v>
       </c>
@@ -17496,20 +17361,8 @@
         <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
         <v>5810700000000</v>
       </c>
-      <c r="AG13">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-      <c r="AH13">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-      <c r="AI13">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>371</v>
       </c>
@@ -17637,20 +17490,8 @@
         <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
         <v>5810700000000</v>
       </c>
-      <c r="AG14">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-      <c r="AH14">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-      <c r="AI14">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>347</v>
       </c>
@@ -17778,20 +17619,8 @@
         <f>About!$A$76*10^6</f>
         <v>3412140000000</v>
       </c>
-      <c r="AG15">
-        <f>About!$A$76*10^6</f>
-        <v>3412140000000</v>
-      </c>
-      <c r="AH15">
-        <f>About!$A$76*10^6</f>
-        <v>3412140000000</v>
-      </c>
-      <c r="AI15">
-        <f>About!$A$76*10^6</f>
-        <v>3412140000000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>344</v>
       </c>
@@ -17888,17 +17717,8 @@
       <c r="AF16">
         <v>0</v>
       </c>
-      <c r="AG16">
-        <v>0</v>
-      </c>
-      <c r="AH16">
-        <v>0</v>
-      </c>
-      <c r="AI16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>330</v>
       </c>
@@ -18026,20 +17846,8 @@
         <f>'GREET1 Fuel_Specs'!$D$69*10^6</f>
         <v>12992301971719.6</v>
       </c>
-      <c r="AG17">
-        <f>'GREET1 Fuel_Specs'!$D$69*10^6</f>
-        <v>12992301971719.6</v>
-      </c>
-      <c r="AH17">
-        <f>'GREET1 Fuel_Specs'!$D$69*10^6</f>
-        <v>12992301971719.6</v>
-      </c>
-      <c r="AI17">
-        <f>'GREET1 Fuel_Specs'!$D$69*10^6</f>
-        <v>12992301971719.6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>367</v>
       </c>
@@ -18167,20 +17975,8 @@
         <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
         <v>5810700000000</v>
       </c>
-      <c r="AG18">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-      <c r="AH18">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-      <c r="AI18">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>368</v>
       </c>
@@ -18308,20 +18104,8 @@
         <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
         <v>5810700000000</v>
       </c>
-      <c r="AG19">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-      <c r="AH19">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-      <c r="AI19">
-        <f>'GREET1 Fuel_Specs'!$D$7*gal_per_barrel*10^6</f>
-        <v>5810700000000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>369</v>
       </c>
@@ -18449,20 +18233,8 @@
         <f>'GREET1 Fuel_Specs'!$D$36*10^6</f>
         <v>91410000000</v>
       </c>
-      <c r="AG20" s="4">
-        <f>'GREET1 Fuel_Specs'!$D$36*10^6</f>
-        <v>91410000000</v>
-      </c>
-      <c r="AH20" s="4">
-        <f>'GREET1 Fuel_Specs'!$D$36*10^6</f>
-        <v>91410000000</v>
-      </c>
-      <c r="AI20" s="4">
-        <f>'GREET1 Fuel_Specs'!$D$36*10^6</f>
-        <v>91410000000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>370</v>
       </c>
@@ -18590,20 +18362,8 @@
         <f>'GREET1 Fuel_Specs'!$D$90*10^6</f>
         <v>13583444584264.561</v>
       </c>
-      <c r="AG21">
-        <f>'GREET1 Fuel_Specs'!$D$90*10^6</f>
-        <v>13583444584264.561</v>
-      </c>
-      <c r="AH21">
-        <f>'GREET1 Fuel_Specs'!$D$90*10^6</f>
-        <v>13583444584264.561</v>
-      </c>
-      <c r="AI21">
-        <f>'GREET1 Fuel_Specs'!$D$90*10^6</f>
-        <v>13583444584264.561</v>
-      </c>
-    </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>366</v>
       </c>
@@ -18728,18 +18488,6 @@
         <v>134509803921.56865</v>
       </c>
       <c r="AF22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
-      </c>
-      <c r="AG22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
-      </c>
-      <c r="AH22" s="181">
-        <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
-        <v>134509803921.56865</v>
-      </c>
-      <c r="AI22" s="181">
         <f>'GREET1 Fuel_Specs'!$D$62/'GREET1 Fuel_Specs'!$E$62*10^9</f>
         <v>134509803921.56865</v>
       </c>
@@ -18760,13 +18508,13 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.86328125" customWidth="1"/>
     <col min="2" max="35" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>405</v>
       </c>
@@ -18873,7 +18621,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>352</v>
       </c>
@@ -19014,7 +18762,7 @@
         <v>3412140</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>323</v>
       </c>
@@ -19155,7 +18903,7 @@
         <v>19887484</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>324</v>
       </c>
@@ -19296,7 +19044,7 @@
         <v>1036999.9999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>358</v>
       </c>
@@ -19437,7 +19185,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>341</v>
       </c>
@@ -19544,7 +19292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>342</v>
       </c>
@@ -19651,7 +19399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>343</v>
       </c>
@@ -19758,7 +19506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>325</v>
       </c>
@@ -19899,7 +19647,7 @@
         <v>17906000</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>326</v>
       </c>
@@ -20040,7 +19788,7 @@
         <v>119596.09523809524</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>327</v>
       </c>
@@ -20181,7 +19929,7 @@
         <v>138690.47619047618</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>328</v>
       </c>
@@ -20322,7 +20070,7 @@
         <v>94981.738095238092</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>329</v>
       </c>
@@ -20463,7 +20211,7 @@
         <v>127595.23809523809</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>371</v>
       </c>
@@ -20604,7 +20352,7 @@
         <v>135000</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>353</v>
       </c>
@@ -20745,7 +20493,7 @@
         <v>3412140</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>344</v>
       </c>
@@ -20852,7 +20600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>330</v>
       </c>
@@ -20993,7 +20741,7 @@
         <v>12992301.9717196</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>367</v>
       </c>
@@ -21134,7 +20882,7 @@
         <v>5810700</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>368</v>
       </c>
@@ -21275,7 +21023,7 @@
         <v>5810700</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>369</v>
       </c>
@@ -21416,7 +21164,7 @@
         <v>91410</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>370</v>
       </c>
@@ -21557,7 +21305,7 @@
         <v>13583444.58426456</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>366</v>
       </c>
@@ -21714,13 +21462,13 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="1" max="1" width="38.26953125" customWidth="1"/>
     <col min="2" max="35" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>403</v>
       </c>
@@ -21827,7 +21575,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>310</v>
       </c>
@@ -21934,7 +21682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>311</v>
       </c>
@@ -22041,7 +21789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>318</v>
       </c>
@@ -22182,7 +21930,7 @@
         <v>119596.09523809524</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>319</v>
       </c>
@@ -22323,7 +22071,7 @@
         <v>138690.47619047618</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>312</v>
       </c>
@@ -22430,7 +22178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>313</v>
       </c>
@@ -22537,7 +22285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>320</v>
       </c>
@@ -22678,7 +22426,7 @@
         <v>135000</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>400</v>
       </c>
@@ -22785,7 +22533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>369</v>
       </c>
@@ -22892,7 +22640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>366</v>
       </c>
@@ -23015,17 +22763,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B1" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>299</v>
       </c>
@@ -23050,23 +22798,23 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A2">
         <f>CONVERT(About!A77,"kg","lbm")*1000000000</f>
         <v>134510640026859.36</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A3" s="182"/>
     </row>
   </sheetData>

</xml_diff>